<commit_message>
StateTL 11/11/2021 GLE moving avg, cal stats, urfthreshold - Issue #7 and #15
</commit_message>
<xml_diff>
--- a/matlab/StateTL_inputdata.xlsx
+++ b/matlab/StateTL_inputdata.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="211">
   <si>
     <t>Reach</t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t>should probably stub out</t>
+  </si>
+  <si>
+    <t>URFThreshold</t>
   </si>
 </sst>
 </file>
@@ -1105,13 +1108,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW78"/>
+  <dimension ref="A1:AX78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,15 +1152,16 @@
     <col min="38" max="39" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="5.5703125" customWidth="1"/>
     <col min="41" max="42" width="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.7109375" customWidth="1"/>
-    <col min="44" max="44" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="6.28515625" customWidth="1"/>
-    <col min="48" max="48" width="6.28515625" style="1" customWidth="1"/>
-    <col min="49" max="49" width="6.28515625" style="14" customWidth="1"/>
+    <col min="43" max="43" width="9" style="2" customWidth="1"/>
+    <col min="44" max="44" width="4.7109375" customWidth="1"/>
+    <col min="45" max="45" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="6.28515625" customWidth="1"/>
+    <col min="49" max="49" width="6.28515625" style="1" customWidth="1"/>
+    <col min="50" max="50" width="6.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1266,29 +1270,32 @@
       <c r="AP1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AQ1" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AR1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AW1" s="13" t="s">
+      <c r="AX1" s="13" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1322,15 +1329,16 @@
       <c r="AN2" s="19"/>
       <c r="AO2" s="19"/>
       <c r="AP2" s="19"/>
-      <c r="AQ2" s="19"/>
+      <c r="AQ2" s="25"/>
       <c r="AR2" s="19"/>
       <c r="AS2" s="19"/>
       <c r="AT2" s="19"/>
       <c r="AU2" s="19"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="19"/>
-    </row>
-    <row r="3" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="19"/>
+    </row>
+    <row r="3" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1442,27 +1450,30 @@
         <v>0.21</v>
       </c>
       <c r="AQ3" s="16">
+        <v>500</v>
+      </c>
+      <c r="AR3" s="16">
         <v>17</v>
       </c>
-      <c r="AR3" s="15">
+      <c r="AS3" s="15">
         <v>10</v>
       </c>
-      <c r="AS3" s="16">
-        <f>AS4</f>
+      <c r="AT3" s="16">
+        <f>AT4</f>
         <v>-999</v>
       </c>
-      <c r="AT3" s="17">
+      <c r="AU3" s="17">
         <v>0.31</v>
       </c>
-      <c r="AU3" s="17">
+      <c r="AV3" s="17">
         <v>1.32</v>
       </c>
-      <c r="AV3" s="17">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="18"/>
-    </row>
-    <row r="4" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="18"/>
+    </row>
+    <row r="4" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1575,26 +1586,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ4" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR4" s="4">
         <v>17</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AS4" s="3">
         <v>10</v>
       </c>
-      <c r="AS4" s="4">
+      <c r="AT4" s="4">
         <v>-999</v>
       </c>
-      <c r="AT4" s="5">
+      <c r="AU4" s="5">
         <v>0.31</v>
       </c>
-      <c r="AU4" s="5">
+      <c r="AV4" s="5">
         <v>1.32</v>
       </c>
-      <c r="AV4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="13"/>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="13"/>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1715,25 +1729,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ5" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR5" s="2">
         <v>17</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>10</v>
       </c>
-      <c r="AS5" s="2">
+      <c r="AT5" s="2">
         <v>110</v>
       </c>
-      <c r="AT5" s="1">
+      <c r="AU5" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU5" s="1">
+      <c r="AV5" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV5" s="1">
+      <c r="AW5" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5</f>
         <v>2</v>
@@ -1854,25 +1871,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ6" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR6" s="2">
         <v>17</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>20</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AT6" s="2">
         <v>110</v>
       </c>
-      <c r="AT6" s="1">
+      <c r="AU6" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU6" s="1">
+      <c r="AV6" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV6" s="1">
+      <c r="AW6" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:C22" si="9">A6</f>
         <v>2</v>
@@ -1987,25 +2007,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ7" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR7" s="2">
         <v>17</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>20</v>
       </c>
-      <c r="AS7" s="2">
+      <c r="AT7" s="2">
         <v>110</v>
       </c>
-      <c r="AT7" s="1">
+      <c r="AU7" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU7" s="1">
+      <c r="AV7" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV7" s="1">
+      <c r="AW7" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -2128,25 +2151,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ8" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR8" s="2">
         <v>17</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <v>20</v>
       </c>
-      <c r="AS8" s="2">
+      <c r="AT8" s="2">
         <v>110</v>
       </c>
-      <c r="AT8" s="1">
+      <c r="AU8" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU8" s="1">
+      <c r="AV8" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV8" s="1">
+      <c r="AW8" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -2260,25 +2286,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ9" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR9" s="2">
         <v>17</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>20</v>
       </c>
-      <c r="AS9" s="2">
+      <c r="AT9" s="2">
         <v>110</v>
       </c>
-      <c r="AT9" s="1">
+      <c r="AU9" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU9" s="1">
+      <c r="AV9" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV9" s="1">
+      <c r="AW9" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -2406,25 +2435,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ10" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR10" s="2">
         <v>17</v>
       </c>
-      <c r="AR10">
+      <c r="AS10">
         <v>20</v>
       </c>
-      <c r="AS10" s="2">
+      <c r="AT10" s="2">
         <v>110</v>
       </c>
-      <c r="AT10" s="1">
+      <c r="AU10" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU10" s="1">
+      <c r="AV10" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV10" s="1">
+      <c r="AW10" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -2536,25 +2568,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ11" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR11" s="2">
         <v>17</v>
       </c>
-      <c r="AR11">
+      <c r="AS11">
         <v>20</v>
       </c>
-      <c r="AS11" s="2">
+      <c r="AT11" s="2">
         <v>110</v>
       </c>
-      <c r="AT11" s="1">
+      <c r="AU11" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU11" s="1">
+      <c r="AV11" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV11" s="1">
+      <c r="AW11" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -2678,25 +2713,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ12" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR12" s="2">
         <v>17</v>
       </c>
-      <c r="AR12">
+      <c r="AS12">
         <v>20</v>
       </c>
-      <c r="AS12" s="2">
+      <c r="AT12" s="2">
         <v>110</v>
       </c>
-      <c r="AT12" s="1">
+      <c r="AU12" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU12" s="1">
+      <c r="AV12" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV12" s="1">
+      <c r="AW12" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -2821,25 +2859,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ13" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR13" s="2">
         <v>17</v>
       </c>
-      <c r="AR13">
+      <c r="AS13">
         <v>20</v>
       </c>
-      <c r="AS13" s="2">
+      <c r="AT13" s="2">
         <v>110</v>
       </c>
-      <c r="AT13" s="1">
+      <c r="AU13" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU13" s="1">
+      <c r="AV13" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV13" s="1">
+      <c r="AW13" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -2958,25 +2999,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ14" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR14" s="2">
         <v>17</v>
       </c>
-      <c r="AR14">
+      <c r="AS14">
         <v>20</v>
       </c>
-      <c r="AS14" s="2">
+      <c r="AT14" s="2">
         <v>110</v>
       </c>
-      <c r="AT14" s="1">
+      <c r="AU14" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU14" s="1">
+      <c r="AV14" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV14" s="1">
+      <c r="AW14" s="1">
         <v>1.17</v>
       </c>
     </row>
-    <row r="15" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -3100,26 +3144,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ15" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR15" s="4">
         <v>17</v>
       </c>
-      <c r="AR15" s="3">
+      <c r="AS15" s="3">
         <v>20</v>
       </c>
-      <c r="AS15" s="4">
+      <c r="AT15" s="4">
         <v>110</v>
       </c>
-      <c r="AT15" s="5">
+      <c r="AU15" s="5">
         <v>0.31</v>
       </c>
-      <c r="AU15" s="5">
+      <c r="AV15" s="5">
         <v>1.32</v>
       </c>
-      <c r="AV15" s="5">
+      <c r="AW15" s="5">
         <v>1.17</v>
       </c>
-      <c r="AW15" s="13"/>
-    </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX15" s="13"/>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -3240,25 +3287,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ16" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR16" s="2">
         <v>17</v>
       </c>
-      <c r="AR16">
+      <c r="AS16">
         <v>20</v>
       </c>
-      <c r="AS16" s="2">
+      <c r="AT16" s="2">
         <v>203</v>
       </c>
-      <c r="AT16" s="1">
+      <c r="AU16" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU16" s="1">
+      <c r="AV16" s="1">
         <v>1.5</v>
       </c>
-      <c r="AV16" s="1">
+      <c r="AW16" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -3375,25 +3425,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ17" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR17" s="2">
         <v>17</v>
       </c>
-      <c r="AR17">
+      <c r="AS17">
         <v>20</v>
       </c>
-      <c r="AS17" s="2">
+      <c r="AT17" s="2">
         <v>203</v>
       </c>
-      <c r="AT17" s="1">
+      <c r="AU17" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU17" s="1">
+      <c r="AV17" s="1">
         <v>1.5</v>
       </c>
-      <c r="AV17" s="1">
+      <c r="AW17" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -3510,25 +3563,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ18" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR18" s="2">
         <v>17</v>
       </c>
-      <c r="AR18">
+      <c r="AS18">
         <v>20</v>
       </c>
-      <c r="AS18" s="2">
+      <c r="AT18" s="2">
         <v>203</v>
       </c>
-      <c r="AT18" s="1">
+      <c r="AU18" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU18" s="1">
+      <c r="AV18" s="1">
         <v>1.5</v>
       </c>
-      <c r="AV18" s="1">
+      <c r="AW18" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -3649,25 +3705,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ19" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR19" s="2">
         <v>17</v>
       </c>
-      <c r="AR19">
+      <c r="AS19">
         <v>20</v>
       </c>
-      <c r="AS19" s="2">
+      <c r="AT19" s="2">
         <v>203</v>
       </c>
-      <c r="AT19" s="1">
+      <c r="AU19" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU19" s="1">
+      <c r="AV19" s="1">
         <v>1.5</v>
       </c>
-      <c r="AV19" s="1">
+      <c r="AW19" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -3788,25 +3847,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ20" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR20" s="2">
         <v>17</v>
       </c>
-      <c r="AR20">
+      <c r="AS20">
         <v>20</v>
       </c>
-      <c r="AS20" s="2">
+      <c r="AT20" s="2">
         <v>203</v>
       </c>
-      <c r="AT20" s="1">
+      <c r="AU20" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU20" s="1">
+      <c r="AV20" s="1">
         <v>1.5</v>
       </c>
-      <c r="AV20" s="1">
+      <c r="AW20" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -3927,25 +3989,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ21" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR21" s="2">
         <v>17</v>
       </c>
-      <c r="AR21">
+      <c r="AS21">
         <v>20</v>
       </c>
-      <c r="AS21" s="2">
+      <c r="AT21" s="2">
         <v>203</v>
       </c>
-      <c r="AT21" s="1">
+      <c r="AU21" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU21" s="1">
+      <c r="AV21" s="1">
         <v>1.5</v>
       </c>
-      <c r="AV21" s="1">
+      <c r="AW21" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="22" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
@@ -4068,26 +4133,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ22" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR22" s="4">
         <v>17</v>
       </c>
-      <c r="AR22" s="3">
+      <c r="AS22" s="3">
         <v>20</v>
       </c>
-      <c r="AS22" s="4">
+      <c r="AT22" s="4">
         <v>203</v>
       </c>
-      <c r="AT22" s="5">
+      <c r="AU22" s="5">
         <v>0.31</v>
       </c>
-      <c r="AU22" s="5">
+      <c r="AV22" s="5">
         <v>1.5</v>
       </c>
-      <c r="AV22" s="5">
+      <c r="AW22" s="5">
         <v>1.05</v>
       </c>
-      <c r="AW22" s="13"/>
-    </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX22" s="13"/>
+    </row>
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ref="A23:C38" si="14">A22</f>
         <v>2</v>
@@ -4208,25 +4276,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ23" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR23" s="2">
         <v>17</v>
       </c>
-      <c r="AR23">
+      <c r="AS23">
         <v>20</v>
       </c>
-      <c r="AS23" s="2">
+      <c r="AT23" s="2">
         <v>85</v>
       </c>
-      <c r="AT23" s="1">
+      <c r="AU23" s="1">
         <v>0.37</v>
       </c>
-      <c r="AU23" s="1">
+      <c r="AV23" s="1">
         <v>1.38</v>
       </c>
-      <c r="AV23" s="1">
+      <c r="AW23" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -4347,25 +4418,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ24" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR24" s="2">
         <v>17</v>
       </c>
-      <c r="AR24">
+      <c r="AS24">
         <v>20</v>
       </c>
-      <c r="AS24" s="2">
+      <c r="AT24" s="2">
         <v>85</v>
       </c>
-      <c r="AT24" s="1">
+      <c r="AU24" s="1">
         <v>0.37</v>
       </c>
-      <c r="AU24" s="1">
+      <c r="AV24" s="1">
         <v>1.38</v>
       </c>
-      <c r="AV24" s="1">
+      <c r="AW24" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -4479,28 +4553,31 @@
         <v>0.21</v>
       </c>
       <c r="AQ25" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR25" s="2">
         <v>17</v>
       </c>
-      <c r="AR25">
+      <c r="AS25">
         <v>20</v>
       </c>
-      <c r="AS25" s="2">
+      <c r="AT25" s="2">
         <v>85</v>
       </c>
-      <c r="AT25" s="1">
+      <c r="AU25" s="1">
         <v>0.37</v>
       </c>
-      <c r="AU25" s="1">
+      <c r="AV25" s="1">
         <v>1.38</v>
       </c>
-      <c r="AV25" s="1">
+      <c r="AW25" s="1">
         <v>1.05</v>
       </c>
-      <c r="AW25" s="14" t="s">
+      <c r="AX25" s="14" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -4627,26 +4704,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ26" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR26" s="4">
         <v>17</v>
       </c>
-      <c r="AR26" s="3">
+      <c r="AS26" s="3">
         <v>20</v>
       </c>
-      <c r="AS26" s="4">
+      <c r="AT26" s="4">
         <v>85</v>
       </c>
-      <c r="AT26" s="5">
+      <c r="AU26" s="5">
         <v>0.37</v>
       </c>
-      <c r="AU26" s="5">
+      <c r="AV26" s="5">
         <v>1.38</v>
       </c>
-      <c r="AV26" s="5">
+      <c r="AW26" s="5">
         <v>1.05</v>
       </c>
-      <c r="AW26" s="13"/>
-    </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX26" s="13"/>
+    </row>
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -4768,25 +4848,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ27" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR27" s="2">
         <v>17</v>
       </c>
-      <c r="AR27">
+      <c r="AS27">
         <v>20</v>
       </c>
-      <c r="AS27" s="2">
+      <c r="AT27" s="2">
         <v>17</v>
       </c>
-      <c r="AT27" s="1">
+      <c r="AU27" s="1">
         <v>0.44</v>
       </c>
-      <c r="AU27" s="1">
+      <c r="AV27" s="1">
         <v>1.18</v>
       </c>
-      <c r="AV27" s="1">
+      <c r="AW27" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -4908,25 +4991,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ28" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR28" s="2">
         <v>17</v>
       </c>
-      <c r="AR28">
+      <c r="AS28">
         <v>20</v>
       </c>
-      <c r="AS28" s="2">
+      <c r="AT28" s="2">
         <v>17</v>
       </c>
-      <c r="AT28" s="1">
+      <c r="AU28" s="1">
         <v>0.44</v>
       </c>
-      <c r="AU28" s="1">
+      <c r="AV28" s="1">
         <v>1.18</v>
       </c>
-      <c r="AV28" s="1">
+      <c r="AW28" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -5051,25 +5137,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ29" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR29" s="2">
         <v>17</v>
       </c>
-      <c r="AR29">
+      <c r="AS29">
         <v>20</v>
       </c>
-      <c r="AS29" s="2">
+      <c r="AT29" s="2">
         <v>17</v>
       </c>
-      <c r="AT29" s="1">
+      <c r="AU29" s="1">
         <v>0.44</v>
       </c>
-      <c r="AU29" s="1">
+      <c r="AV29" s="1">
         <v>1.18</v>
       </c>
-      <c r="AV29" s="1">
+      <c r="AW29" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -5189,25 +5278,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ30" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR30" s="2">
         <v>17</v>
       </c>
-      <c r="AR30">
+      <c r="AS30">
         <v>20</v>
       </c>
-      <c r="AS30" s="2">
+      <c r="AT30" s="2">
         <v>17</v>
       </c>
-      <c r="AT30" s="1">
+      <c r="AU30" s="1">
         <v>0.44</v>
       </c>
-      <c r="AU30" s="1">
+      <c r="AV30" s="1">
         <v>1.18</v>
       </c>
-      <c r="AV30" s="1">
+      <c r="AW30" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -5327,25 +5419,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ31" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR31" s="2">
         <v>17</v>
       </c>
-      <c r="AR31">
+      <c r="AS31">
         <v>20</v>
       </c>
-      <c r="AS31" s="2">
+      <c r="AT31" s="2">
         <v>17</v>
       </c>
-      <c r="AT31" s="1">
+      <c r="AU31" s="1">
         <v>0.44</v>
       </c>
-      <c r="AU31" s="1">
+      <c r="AV31" s="1">
         <v>1.18</v>
       </c>
-      <c r="AV31" s="1">
+      <c r="AW31" s="1">
         <v>1.05</v>
       </c>
     </row>
-    <row r="32" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -5476,26 +5571,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ32" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR32" s="4">
         <v>17</v>
       </c>
-      <c r="AR32" s="3">
+      <c r="AS32" s="3">
         <v>20</v>
       </c>
-      <c r="AS32" s="4">
+      <c r="AT32" s="4">
         <v>17</v>
       </c>
-      <c r="AT32" s="5">
+      <c r="AU32" s="5">
         <v>0.44</v>
       </c>
-      <c r="AU32" s="5">
+      <c r="AV32" s="5">
         <v>1.18</v>
       </c>
-      <c r="AV32" s="5">
+      <c r="AW32" s="5">
         <v>1.05</v>
       </c>
-      <c r="AW32" s="13"/>
-    </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX32" s="13"/>
+    </row>
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -5621,25 +5719,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ33" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR33" s="2">
         <v>17</v>
       </c>
-      <c r="AR33">
+      <c r="AS33">
         <v>20</v>
       </c>
-      <c r="AS33" s="2">
+      <c r="AT33" s="2">
         <v>56</v>
       </c>
-      <c r="AT33" s="1">
+      <c r="AU33" s="1">
         <v>0.49</v>
       </c>
-      <c r="AU33" s="1">
+      <c r="AV33" s="1">
         <v>0.96</v>
       </c>
-      <c r="AV33" s="1">
+      <c r="AW33" s="1">
         <v>1.04</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -5755,28 +5856,31 @@
         <v>0.21</v>
       </c>
       <c r="AQ34" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR34" s="2">
         <v>17</v>
       </c>
-      <c r="AR34">
+      <c r="AS34">
         <v>20</v>
       </c>
-      <c r="AS34" s="2">
+      <c r="AT34" s="2">
         <v>56</v>
       </c>
-      <c r="AT34" s="1">
+      <c r="AU34" s="1">
         <v>0.49</v>
       </c>
-      <c r="AU34" s="1">
+      <c r="AV34" s="1">
         <v>0.96</v>
       </c>
-      <c r="AV34" s="1">
+      <c r="AW34" s="1">
         <v>1.04</v>
       </c>
-      <c r="AW34" s="14" t="s">
+      <c r="AX34" s="14" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -5907,25 +6011,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ35" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR35" s="2">
         <v>17</v>
       </c>
-      <c r="AR35">
+      <c r="AS35">
         <v>20</v>
       </c>
-      <c r="AS35" s="2">
+      <c r="AT35" s="2">
         <v>56</v>
       </c>
-      <c r="AT35" s="1">
+      <c r="AU35" s="1">
         <v>0.49</v>
       </c>
-      <c r="AU35" s="1">
+      <c r="AV35" s="1">
         <v>0.96</v>
       </c>
-      <c r="AV35" s="1">
+      <c r="AW35" s="1">
         <v>1.04</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -6047,25 +6154,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ36" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR36" s="2">
         <v>17</v>
       </c>
-      <c r="AR36">
+      <c r="AS36">
         <v>20</v>
       </c>
-      <c r="AS36" s="2">
+      <c r="AT36" s="2">
         <v>56</v>
       </c>
-      <c r="AT36" s="1">
+      <c r="AU36" s="1">
         <v>0.49</v>
       </c>
-      <c r="AU36" s="1">
+      <c r="AV36" s="1">
         <v>0.96</v>
       </c>
-      <c r="AV36" s="1">
+      <c r="AW36" s="1">
         <v>1.04</v>
       </c>
     </row>
-    <row r="37" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -6185,28 +6295,31 @@
         <v>0.21</v>
       </c>
       <c r="AQ37" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR37" s="4">
         <v>17</v>
       </c>
-      <c r="AR37" s="3">
+      <c r="AS37" s="3">
         <v>20</v>
       </c>
-      <c r="AS37" s="4">
+      <c r="AT37" s="4">
         <v>56</v>
       </c>
-      <c r="AT37" s="5">
+      <c r="AU37" s="5">
         <v>0.49</v>
       </c>
-      <c r="AU37" s="5">
+      <c r="AV37" s="5">
         <v>0.96</v>
       </c>
-      <c r="AV37" s="5">
+      <c r="AW37" s="5">
         <v>1.04</v>
       </c>
-      <c r="AW37" s="13" t="s">
+      <c r="AX37" s="13" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="14"/>
         <v>2</v>
@@ -6326,25 +6439,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ38" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR38" s="2">
         <v>17</v>
       </c>
-      <c r="AR38">
+      <c r="AS38">
         <v>30</v>
       </c>
-      <c r="AS38" s="2">
+      <c r="AT38" s="2">
         <v>116</v>
       </c>
-      <c r="AT38" s="1">
+      <c r="AU38" s="1">
         <v>0.41</v>
       </c>
-      <c r="AU38" s="1">
+      <c r="AV38" s="1">
         <v>1.06</v>
       </c>
-      <c r="AV38" s="1">
+      <c r="AW38" s="1">
         <v>1.02</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" ref="A39:C43" si="23">A38</f>
         <v>2</v>
@@ -6461,25 +6577,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ39" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR39" s="2">
         <v>17</v>
       </c>
-      <c r="AR39">
+      <c r="AS39">
         <v>40</v>
       </c>
-      <c r="AS39" s="2">
+      <c r="AT39" s="2">
         <v>116</v>
       </c>
-      <c r="AT39" s="1">
+      <c r="AU39" s="1">
         <v>0.41</v>
       </c>
-      <c r="AU39" s="1">
+      <c r="AV39" s="1">
         <v>1.06</v>
       </c>
-      <c r="AV39" s="1">
+      <c r="AW39" s="1">
         <v>1.02</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="23"/>
         <v>2</v>
@@ -6600,25 +6719,28 @@
         <v>0.21</v>
       </c>
       <c r="AQ40" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR40" s="2">
         <v>17</v>
       </c>
-      <c r="AR40">
+      <c r="AS40">
         <v>30</v>
       </c>
-      <c r="AS40" s="2">
+      <c r="AT40" s="2">
         <v>116</v>
       </c>
-      <c r="AT40" s="1">
+      <c r="AU40" s="1">
         <v>0.41</v>
       </c>
-      <c r="AU40" s="1">
+      <c r="AV40" s="1">
         <v>1.06</v>
       </c>
-      <c r="AV40" s="1">
+      <c r="AW40" s="1">
         <v>1.02</v>
       </c>
     </row>
-    <row r="41" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <f t="shared" si="23"/>
         <v>2</v>
@@ -6741,26 +6863,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ41" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR41" s="4">
         <v>17</v>
       </c>
-      <c r="AR41" s="3">
+      <c r="AS41" s="3">
         <v>25</v>
       </c>
-      <c r="AS41" s="4">
+      <c r="AT41" s="4">
         <v>116</v>
       </c>
-      <c r="AT41" s="5">
+      <c r="AU41" s="5">
         <v>0.41</v>
       </c>
-      <c r="AU41" s="5">
+      <c r="AV41" s="5">
         <v>1.06</v>
       </c>
-      <c r="AV41" s="5">
+      <c r="AW41" s="5">
         <v>1.02</v>
       </c>
-      <c r="AW41" s="13"/>
-    </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX41" s="13"/>
+    </row>
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="23"/>
         <v>2</v>
@@ -6881,26 +7006,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ42" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR42" s="2">
         <v>17</v>
       </c>
-      <c r="AR42">
+      <c r="AS42">
         <v>25</v>
       </c>
-      <c r="AS42" s="2">
-        <f>ROUND(AS41*SUM(AA42:AA43)/SUM(AA38:AA41),0)</f>
+      <c r="AT42" s="2">
+        <f>ROUND(AT41*SUM(AA42:AA43)/SUM(AA38:AA41),0)</f>
         <v>29</v>
       </c>
-      <c r="AT42" s="1">
+      <c r="AU42" s="1">
         <v>0.41</v>
       </c>
-      <c r="AU42" s="1">
+      <c r="AV42" s="1">
         <v>1.06</v>
       </c>
-      <c r="AV42" s="1">
+      <c r="AW42" s="1">
         <v>1.01</v>
       </c>
     </row>
-    <row r="43" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f t="shared" si="23"/>
         <v>2</v>
@@ -7023,27 +7151,30 @@
         <v>0.21</v>
       </c>
       <c r="AQ43" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR43" s="4">
         <v>17</v>
       </c>
-      <c r="AR43" s="3">
+      <c r="AS43" s="3">
         <v>25</v>
       </c>
-      <c r="AS43" s="4">
-        <f>AS42</f>
+      <c r="AT43" s="4">
+        <f>AT42</f>
         <v>29</v>
       </c>
-      <c r="AT43" s="5">
+      <c r="AU43" s="5">
         <v>0.41</v>
       </c>
-      <c r="AU43" s="5">
+      <c r="AV43" s="5">
         <v>1.06</v>
       </c>
-      <c r="AV43" s="5">
+      <c r="AW43" s="5">
         <v>1.01</v>
       </c>
-      <c r="AW43" s="13"/>
-    </row>
-    <row r="44" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX43" s="13"/>
+    </row>
+    <row r="44" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
@@ -7078,14 +7209,15 @@
       <c r="AO44" s="19"/>
       <c r="AP44" s="19"/>
       <c r="AQ44" s="25"/>
-      <c r="AR44" s="19"/>
+      <c r="AR44" s="25"/>
       <c r="AS44" s="19"/>
       <c r="AT44" s="19"/>
       <c r="AU44" s="19"/>
-      <c r="AV44" s="20"/>
-      <c r="AW44" s="19"/>
-    </row>
-    <row r="45" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AV44" s="19"/>
+      <c r="AW44" s="20"/>
+      <c r="AX44" s="19"/>
+    </row>
+    <row r="45" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>2</v>
       </c>
@@ -7194,28 +7326,31 @@
         <v>0.21</v>
       </c>
       <c r="AQ45" s="16">
+        <v>500</v>
+      </c>
+      <c r="AR45" s="16">
         <v>17</v>
       </c>
-      <c r="AR45" s="15">
+      <c r="AS45" s="15">
         <v>50</v>
       </c>
-      <c r="AS45" s="16">
+      <c r="AT45" s="16">
         <v>10</v>
       </c>
-      <c r="AT45" s="17">
+      <c r="AU45" s="17">
         <v>0.31</v>
       </c>
-      <c r="AU45" s="17">
+      <c r="AV45" s="17">
         <v>1.32</v>
       </c>
-      <c r="AV45" s="17">
-        <v>0</v>
-      </c>
-      <c r="AW45" s="18" t="s">
+      <c r="AW45" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX45" s="18" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <f t="shared" ref="A46" si="24">A45</f>
         <v>2</v>
@@ -7324,28 +7459,31 @@
         <v>0.21</v>
       </c>
       <c r="AQ46" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR46" s="4">
         <v>17</v>
       </c>
-      <c r="AR46" s="3">
+      <c r="AS46" s="3">
         <v>50</v>
       </c>
-      <c r="AS46" s="4">
+      <c r="AT46" s="4">
         <v>10</v>
       </c>
-      <c r="AT46" s="5">
+      <c r="AU46" s="5">
         <v>0.31</v>
       </c>
-      <c r="AU46" s="5">
+      <c r="AV46" s="5">
         <v>1.32</v>
       </c>
-      <c r="AV46" s="5">
-        <v>0</v>
-      </c>
-      <c r="AW46" s="13" t="s">
+      <c r="AW46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX46" s="13" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
@@ -7373,13 +7511,14 @@
       <c r="AO47" s="21"/>
       <c r="AP47" s="21"/>
       <c r="AQ47" s="7"/>
-      <c r="AS47" s="7"/>
-      <c r="AT47" s="21"/>
+      <c r="AR47" s="7"/>
+      <c r="AT47" s="7"/>
       <c r="AU47" s="21"/>
       <c r="AV47" s="21"/>
-      <c r="AW47" s="22"/>
-    </row>
-    <row r="48" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW47" s="21"/>
+      <c r="AX47" s="22"/>
+    </row>
+    <row r="48" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>2</v>
       </c>
@@ -7499,28 +7638,31 @@
         <v>0.21</v>
       </c>
       <c r="AQ48" s="16">
+        <v>500</v>
+      </c>
+      <c r="AR48" s="16">
         <v>17</v>
       </c>
-      <c r="AR48" s="15">
+      <c r="AS48" s="15">
         <v>50</v>
       </c>
-      <c r="AS48" s="16">
+      <c r="AT48" s="16">
         <v>10</v>
       </c>
-      <c r="AT48" s="17">
+      <c r="AU48" s="17">
         <v>0.31</v>
       </c>
-      <c r="AU48" s="17">
+      <c r="AV48" s="17">
         <v>1.32</v>
       </c>
-      <c r="AV48" s="17">
-        <v>0</v>
-      </c>
-      <c r="AW48" s="18" t="s">
+      <c r="AW48" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX48" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -7634,28 +7776,31 @@
         <v>0.21</v>
       </c>
       <c r="AQ49" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR49" s="2">
         <v>17</v>
       </c>
-      <c r="AR49">
+      <c r="AS49">
         <v>50</v>
       </c>
-      <c r="AS49" s="2">
+      <c r="AT49" s="2">
         <v>10</v>
       </c>
-      <c r="AT49" s="1">
+      <c r="AU49" s="1">
         <v>0.31</v>
       </c>
-      <c r="AU49" s="1">
+      <c r="AV49" s="1">
         <v>1.32</v>
       </c>
-      <c r="AV49" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW49" s="14" t="s">
+      <c r="AW49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX49" s="14" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>2</v>
       </c>
@@ -7769,26 +7914,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ50" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR50" s="4">
         <v>17</v>
       </c>
-      <c r="AR50" s="3">
+      <c r="AS50" s="3">
         <v>50</v>
       </c>
-      <c r="AS50" s="4">
+      <c r="AT50" s="4">
         <v>10</v>
       </c>
-      <c r="AT50" s="5">
+      <c r="AU50" s="5">
         <v>0.31</v>
       </c>
-      <c r="AU50" s="5">
+      <c r="AV50" s="5">
         <v>1.32</v>
       </c>
-      <c r="AV50" s="5">
-        <v>0</v>
-      </c>
-      <c r="AW50" s="13"/>
-    </row>
-    <row r="51" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX50" s="13"/>
+    </row>
+    <row r="51" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -7816,13 +7964,14 @@
       <c r="AO51" s="21"/>
       <c r="AP51" s="21"/>
       <c r="AQ51" s="7"/>
-      <c r="AS51" s="7"/>
-      <c r="AT51" s="21"/>
+      <c r="AR51" s="7"/>
+      <c r="AT51" s="7"/>
       <c r="AU51" s="21"/>
       <c r="AV51" s="21"/>
-      <c r="AW51" s="22"/>
-    </row>
-    <row r="52" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW51" s="21"/>
+      <c r="AX51" s="22"/>
+    </row>
+    <row r="52" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>2</v>
       </c>
@@ -7930,26 +8079,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ52" s="16">
+        <v>500</v>
+      </c>
+      <c r="AR52" s="16">
         <v>17</v>
       </c>
-      <c r="AR52" s="15">
+      <c r="AS52" s="15">
         <v>50</v>
       </c>
-      <c r="AS52" s="16">
+      <c r="AT52" s="16">
         <v>10</v>
       </c>
-      <c r="AT52" s="17">
+      <c r="AU52" s="17">
         <v>0.31</v>
       </c>
-      <c r="AU52" s="17">
+      <c r="AV52" s="17">
         <v>1.32</v>
       </c>
-      <c r="AV52" s="17">
+      <c r="AW52" s="17">
         <v>1.27</v>
       </c>
-      <c r="AW52" s="18"/>
-    </row>
-    <row r="53" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX52" s="18"/>
+    </row>
+    <row r="53" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>2</v>
       </c>
@@ -8061,26 +8213,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ53" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR53" s="4">
         <v>17</v>
       </c>
-      <c r="AR53" s="3">
+      <c r="AS53" s="3">
         <v>50</v>
       </c>
-      <c r="AS53" s="4">
+      <c r="AT53" s="4">
         <v>10</v>
       </c>
-      <c r="AT53" s="5">
+      <c r="AU53" s="5">
         <v>0.31</v>
       </c>
-      <c r="AU53" s="5">
+      <c r="AV53" s="5">
         <v>1.32</v>
       </c>
-      <c r="AV53" s="5">
+      <c r="AW53" s="5">
         <v>1.27</v>
       </c>
-      <c r="AW53" s="13"/>
-    </row>
-    <row r="54" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX53" s="13"/>
+    </row>
+    <row r="54" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -8115,14 +8270,15 @@
       <c r="AO54" s="19"/>
       <c r="AP54" s="19"/>
       <c r="AQ54" s="25"/>
-      <c r="AR54" s="19"/>
+      <c r="AR54" s="25"/>
       <c r="AS54" s="19"/>
       <c r="AT54" s="19"/>
       <c r="AU54" s="19"/>
-      <c r="AV54" s="20"/>
-      <c r="AW54" s="19"/>
-    </row>
-    <row r="55" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AV54" s="19"/>
+      <c r="AW54" s="20"/>
+      <c r="AX54" s="19"/>
+    </row>
+    <row r="55" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>2</v>
       </c>
@@ -8217,26 +8373,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ55" s="16">
+        <v>500</v>
+      </c>
+      <c r="AR55" s="16">
         <v>17</v>
       </c>
-      <c r="AR55" s="15">
+      <c r="AS55" s="15">
         <v>50</v>
       </c>
-      <c r="AS55" s="16">
+      <c r="AT55" s="16">
         <v>10</v>
       </c>
-      <c r="AT55" s="17">
+      <c r="AU55" s="17">
         <v>0.31</v>
       </c>
-      <c r="AU55" s="17">
+      <c r="AV55" s="17">
         <v>1.32</v>
       </c>
-      <c r="AV55" s="17">
+      <c r="AW55" s="17">
         <v>1.27</v>
       </c>
-      <c r="AW55" s="18"/>
-    </row>
-    <row r="56" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX55" s="18"/>
+    </row>
+    <row r="56" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>2</v>
       </c>
@@ -8330,26 +8489,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ56" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR56" s="7">
         <v>17</v>
       </c>
-      <c r="AR56" s="6">
+      <c r="AS56" s="6">
         <v>50</v>
       </c>
-      <c r="AS56" s="7">
+      <c r="AT56" s="7">
         <v>10</v>
       </c>
-      <c r="AT56" s="21">
+      <c r="AU56" s="21">
         <v>0.31</v>
       </c>
-      <c r="AU56" s="21">
+      <c r="AV56" s="21">
         <v>1.32</v>
       </c>
-      <c r="AV56" s="21">
+      <c r="AW56" s="21">
         <v>1.17</v>
       </c>
-      <c r="AW56" s="22"/>
-    </row>
-    <row r="57" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX56" s="22"/>
+    </row>
+    <row r="57" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>2</v>
       </c>
@@ -8447,26 +8609,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ57" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR57" s="4">
         <v>17</v>
       </c>
-      <c r="AR57" s="3">
+      <c r="AS57" s="3">
         <v>50</v>
       </c>
-      <c r="AS57" s="4">
+      <c r="AT57" s="4">
         <v>10</v>
       </c>
-      <c r="AT57" s="5">
+      <c r="AU57" s="5">
         <v>0.31</v>
       </c>
-      <c r="AU57" s="5">
+      <c r="AV57" s="5">
         <v>1.32</v>
       </c>
-      <c r="AV57" s="5">
+      <c r="AW57" s="5">
         <v>1.17</v>
       </c>
-      <c r="AW57" s="13"/>
-    </row>
-    <row r="58" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX57" s="13"/>
+    </row>
+    <row r="58" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F58" s="7"/>
       <c r="H58" s="7"/>
       <c r="Q58" s="30"/>
@@ -8488,11 +8653,12 @@
       <c r="AD58" s="30"/>
       <c r="AE58" s="30"/>
       <c r="AQ58" s="7"/>
-      <c r="AS58" s="7"/>
-      <c r="AV58" s="21"/>
-      <c r="AW58" s="22"/>
-    </row>
-    <row r="59" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AR58" s="7"/>
+      <c r="AT58" s="7"/>
+      <c r="AW58" s="21"/>
+      <c r="AX58" s="22"/>
+    </row>
+    <row r="59" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>2</v>
       </c>
@@ -8606,26 +8772,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ59" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR59" s="7">
         <v>17</v>
       </c>
-      <c r="AR59" s="6">
+      <c r="AS59" s="6">
         <v>50</v>
       </c>
-      <c r="AS59" s="7">
+      <c r="AT59" s="7">
         <v>110</v>
       </c>
-      <c r="AT59" s="6">
+      <c r="AU59" s="6">
         <v>0.31</v>
       </c>
-      <c r="AU59" s="6">
+      <c r="AV59" s="6">
         <v>1.32</v>
       </c>
-      <c r="AV59" s="21">
+      <c r="AW59" s="21">
         <v>1.27</v>
       </c>
-      <c r="AW59" s="22"/>
-    </row>
-    <row r="60" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX59" s="22"/>
+    </row>
+    <row r="60" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>2</v>
       </c>
@@ -8735,26 +8904,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ60" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR60" s="7">
         <v>17</v>
       </c>
-      <c r="AR60" s="6">
+      <c r="AS60" s="6">
         <v>50</v>
       </c>
-      <c r="AS60" s="7">
+      <c r="AT60" s="7">
         <v>110</v>
       </c>
-      <c r="AT60" s="6">
+      <c r="AU60" s="6">
         <v>0.31</v>
       </c>
-      <c r="AU60" s="6">
+      <c r="AV60" s="6">
         <v>1.32</v>
       </c>
-      <c r="AV60" s="21">
+      <c r="AW60" s="21">
         <v>1.27</v>
       </c>
-      <c r="AW60" s="22"/>
-    </row>
-    <row r="61" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX60" s="22"/>
+    </row>
+    <row r="61" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>2</v>
       </c>
@@ -8864,26 +9036,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ61" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR61" s="7">
         <v>17</v>
       </c>
-      <c r="AR61" s="6">
+      <c r="AS61" s="6">
         <v>50</v>
       </c>
-      <c r="AS61" s="7">
+      <c r="AT61" s="7">
         <v>110</v>
       </c>
-      <c r="AT61" s="6">
+      <c r="AU61" s="6">
         <v>0.31</v>
       </c>
-      <c r="AU61" s="6">
+      <c r="AV61" s="6">
         <v>1.32</v>
       </c>
-      <c r="AV61" s="21">
+      <c r="AW61" s="21">
         <v>1.27</v>
       </c>
-      <c r="AW61" s="22"/>
-    </row>
-    <row r="62" spans="1:49" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX61" s="22"/>
+    </row>
+    <row r="62" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>2</v>
       </c>
@@ -8993,26 +9168,29 @@
         <v>0.21</v>
       </c>
       <c r="AQ62" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR62" s="4">
         <v>17</v>
       </c>
-      <c r="AR62" s="3">
+      <c r="AS62" s="3">
         <v>50</v>
       </c>
-      <c r="AS62" s="4">
+      <c r="AT62" s="4">
         <v>110</v>
       </c>
-      <c r="AT62" s="3">
+      <c r="AU62" s="3">
         <v>0.31</v>
       </c>
-      <c r="AU62" s="3">
+      <c r="AV62" s="3">
         <v>1.32</v>
       </c>
-      <c r="AV62" s="5">
+      <c r="AW62" s="5">
         <v>1.27</v>
       </c>
-      <c r="AW62" s="13"/>
-    </row>
-    <row r="64" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX62" s="13"/>
+    </row>
+    <row r="64" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -9111,27 +9289,30 @@
       <c r="AP64">
         <v>0.21</v>
       </c>
-      <c r="AQ64">
+      <c r="AQ64" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR64">
         <v>671</v>
       </c>
-      <c r="AR64">
+      <c r="AS64">
         <v>20</v>
       </c>
-      <c r="AS64" s="2">
+      <c r="AT64" s="2">
         <v>-999</v>
       </c>
-      <c r="AT64">
+      <c r="AU64">
         <v>0.38</v>
       </c>
-      <c r="AU64">
+      <c r="AV64">
         <v>0.99</v>
       </c>
-      <c r="AV64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW64" s="14"/>
-    </row>
-    <row r="65" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX64" s="14"/>
+    </row>
+    <row r="65" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>2</v>
       </c>
@@ -9229,27 +9410,30 @@
       <c r="AP65" s="15">
         <v>0.21</v>
       </c>
-      <c r="AQ65" s="15">
+      <c r="AQ65" s="16">
+        <v>500</v>
+      </c>
+      <c r="AR65" s="15">
         <v>671</v>
       </c>
-      <c r="AR65" s="15">
+      <c r="AS65" s="15">
         <v>50</v>
       </c>
-      <c r="AS65" s="18">
+      <c r="AT65" s="18">
         <v>10.7</v>
       </c>
-      <c r="AT65" s="15">
+      <c r="AU65" s="15">
         <v>0.38</v>
       </c>
-      <c r="AU65" s="15">
+      <c r="AV65" s="15">
         <v>0.99</v>
       </c>
-      <c r="AV65" s="17">
-        <v>1</v>
-      </c>
-      <c r="AW65" s="18"/>
-    </row>
-    <row r="66" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW65" s="17">
+        <v>1</v>
+      </c>
+      <c r="AX65" s="18"/>
+    </row>
+    <row r="66" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>2</v>
       </c>
@@ -9349,27 +9533,30 @@
       <c r="AP66" s="6">
         <v>0.21</v>
       </c>
-      <c r="AQ66" s="6">
+      <c r="AQ66" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR66" s="6">
         <v>671</v>
       </c>
-      <c r="AR66" s="6">
+      <c r="AS66" s="6">
         <v>50</v>
       </c>
-      <c r="AS66" s="22">
+      <c r="AT66" s="22">
         <v>10.7</v>
       </c>
-      <c r="AT66" s="6">
+      <c r="AU66" s="6">
         <v>0.38</v>
       </c>
-      <c r="AU66" s="6">
+      <c r="AV66" s="6">
         <v>0.99</v>
       </c>
-      <c r="AV66" s="21">
-        <v>1</v>
-      </c>
-      <c r="AW66" s="22"/>
-    </row>
-    <row r="67" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW66" s="21">
+        <v>1</v>
+      </c>
+      <c r="AX66" s="22"/>
+    </row>
+    <row r="67" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>2</v>
       </c>
@@ -9463,27 +9650,30 @@
       <c r="AP67" s="6">
         <v>0.21</v>
       </c>
-      <c r="AQ67" s="6">
+      <c r="AQ67" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR67" s="6">
         <v>671</v>
       </c>
-      <c r="AR67" s="6">
+      <c r="AS67" s="6">
         <v>50</v>
       </c>
-      <c r="AS67" s="22">
+      <c r="AT67" s="22">
         <v>10.7</v>
       </c>
-      <c r="AT67" s="6">
+      <c r="AU67" s="6">
         <v>0.38</v>
       </c>
-      <c r="AU67" s="6">
+      <c r="AV67" s="6">
         <v>0.99</v>
       </c>
-      <c r="AV67" s="21">
-        <v>1</v>
-      </c>
-      <c r="AW67" s="22"/>
-    </row>
-    <row r="68" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW67" s="21">
+        <v>1</v>
+      </c>
+      <c r="AX67" s="22"/>
+    </row>
+    <row r="68" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>2</v>
       </c>
@@ -9607,27 +9797,30 @@
       <c r="AP68" s="6">
         <v>0.21</v>
       </c>
-      <c r="AQ68" s="6">
+      <c r="AQ68" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR68" s="6">
         <v>671</v>
       </c>
-      <c r="AR68" s="6">
+      <c r="AS68" s="6">
         <v>50</v>
       </c>
-      <c r="AS68" s="22">
+      <c r="AT68" s="22">
         <v>10.7</v>
       </c>
-      <c r="AT68" s="6">
+      <c r="AU68" s="6">
         <v>0.38</v>
       </c>
-      <c r="AU68" s="6">
+      <c r="AV68" s="6">
         <v>0.99</v>
       </c>
-      <c r="AV68" s="21">
-        <v>1</v>
-      </c>
-      <c r="AW68" s="22"/>
-    </row>
-    <row r="69" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW68" s="21">
+        <v>1</v>
+      </c>
+      <c r="AX68" s="22"/>
+    </row>
+    <row r="69" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>2</v>
       </c>
@@ -9744,27 +9937,30 @@
       <c r="AP69" s="3">
         <v>0.21</v>
       </c>
-      <c r="AQ69" s="3">
+      <c r="AQ69" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR69" s="3">
         <v>671</v>
       </c>
-      <c r="AR69" s="3">
+      <c r="AS69" s="3">
         <v>50</v>
       </c>
-      <c r="AS69" s="13">
+      <c r="AT69" s="13">
         <v>10.7</v>
       </c>
-      <c r="AT69" s="3">
+      <c r="AU69" s="3">
         <v>0.38</v>
       </c>
-      <c r="AU69" s="3">
+      <c r="AV69" s="3">
         <v>0.99</v>
       </c>
-      <c r="AV69" s="5">
-        <v>1</v>
-      </c>
-      <c r="AW69" s="13"/>
-    </row>
-    <row r="70" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW69" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX69" s="13"/>
+    </row>
+    <row r="70" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2</v>
       </c>
@@ -9864,26 +10060,29 @@
       <c r="AP70">
         <v>0.21</v>
       </c>
-      <c r="AQ70">
+      <c r="AQ70" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR70">
         <v>673</v>
       </c>
-      <c r="AR70">
+      <c r="AS70">
         <v>50</v>
       </c>
-      <c r="AS70" s="18">
+      <c r="AT70" s="18">
         <v>29.7</v>
       </c>
-      <c r="AT70">
+      <c r="AU70">
         <v>0.38</v>
       </c>
-      <c r="AU70">
+      <c r="AV70">
         <v>0.99</v>
       </c>
-      <c r="AV70" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2</v>
       </c>
@@ -9981,26 +10180,29 @@
       <c r="AP71">
         <v>0.21</v>
       </c>
-      <c r="AQ71">
+      <c r="AQ71" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR71">
         <v>673</v>
       </c>
-      <c r="AR71">
+      <c r="AS71">
         <v>50</v>
       </c>
-      <c r="AS71" s="14">
+      <c r="AT71" s="14">
         <v>29.7</v>
       </c>
-      <c r="AT71">
+      <c r="AU71">
         <v>0.38</v>
       </c>
-      <c r="AU71">
+      <c r="AV71">
         <v>0.99</v>
       </c>
-      <c r="AV71" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2</v>
       </c>
@@ -10098,26 +10300,29 @@
       <c r="AP72">
         <v>0.21</v>
       </c>
-      <c r="AQ72">
+      <c r="AQ72" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR72">
         <v>673</v>
       </c>
-      <c r="AR72">
+      <c r="AS72">
         <v>50</v>
       </c>
-      <c r="AS72" s="14">
+      <c r="AT72" s="14">
         <v>29.7</v>
       </c>
-      <c r="AT72">
+      <c r="AU72">
         <v>0.38</v>
       </c>
-      <c r="AU72">
+      <c r="AV72">
         <v>0.99</v>
       </c>
-      <c r="AV72" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2</v>
       </c>
@@ -10209,26 +10414,29 @@
       <c r="AP73">
         <v>0.21</v>
       </c>
-      <c r="AQ73">
+      <c r="AQ73" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR73">
         <v>673</v>
       </c>
-      <c r="AR73">
+      <c r="AS73">
         <v>50</v>
       </c>
-      <c r="AS73" s="14">
+      <c r="AT73" s="14">
         <v>29.7</v>
       </c>
-      <c r="AT73">
+      <c r="AU73">
         <v>0.38</v>
       </c>
-      <c r="AU73">
+      <c r="AV73">
         <v>0.99</v>
       </c>
-      <c r="AV73" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2</v>
       </c>
@@ -10326,26 +10534,29 @@
       <c r="AP74">
         <v>0.21</v>
       </c>
-      <c r="AQ74">
+      <c r="AQ74" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR74">
         <v>673</v>
       </c>
-      <c r="AR74">
+      <c r="AS74">
         <v>50</v>
       </c>
-      <c r="AS74" s="14">
+      <c r="AT74" s="14">
         <v>29.7</v>
       </c>
-      <c r="AT74">
+      <c r="AU74">
         <v>0.38</v>
       </c>
-      <c r="AU74">
+      <c r="AV74">
         <v>0.99</v>
       </c>
-      <c r="AV74" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <v>2</v>
       </c>
@@ -10444,27 +10655,30 @@
       <c r="AP75" s="15">
         <v>0.21</v>
       </c>
-      <c r="AQ75" s="15">
+      <c r="AQ75" s="16">
+        <v>500</v>
+      </c>
+      <c r="AR75" s="15">
         <v>674</v>
       </c>
-      <c r="AR75" s="15">
+      <c r="AS75" s="15">
         <v>50</v>
       </c>
-      <c r="AS75" s="18">
+      <c r="AT75" s="18">
         <v>12.4</v>
       </c>
-      <c r="AT75" s="15">
+      <c r="AU75" s="15">
         <v>0.38</v>
       </c>
-      <c r="AU75" s="15">
+      <c r="AV75" s="15">
         <v>0.99</v>
       </c>
-      <c r="AV75" s="17">
-        <v>1</v>
-      </c>
-      <c r="AW75" s="18"/>
-    </row>
-    <row r="76" spans="1:49" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW75" s="17">
+        <v>1</v>
+      </c>
+      <c r="AX75" s="18"/>
+    </row>
+    <row r="76" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>2</v>
       </c>
@@ -10558,27 +10772,30 @@
       <c r="AP76" s="6">
         <v>0.21</v>
       </c>
-      <c r="AQ76" s="6">
+      <c r="AQ76" s="7">
+        <v>500</v>
+      </c>
+      <c r="AR76" s="6">
         <v>674</v>
       </c>
-      <c r="AR76" s="6">
+      <c r="AS76" s="6">
         <v>50</v>
       </c>
-      <c r="AS76" s="22">
+      <c r="AT76" s="22">
         <v>12.4</v>
       </c>
-      <c r="AT76" s="6">
+      <c r="AU76" s="6">
         <v>0.38</v>
       </c>
-      <c r="AU76" s="6">
+      <c r="AV76" s="6">
         <v>0.99</v>
       </c>
-      <c r="AV76" s="21">
-        <v>1</v>
-      </c>
-      <c r="AW76" s="22"/>
-    </row>
-    <row r="77" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AW76" s="21">
+        <v>1</v>
+      </c>
+      <c r="AX76" s="22"/>
+    </row>
+    <row r="77" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>2</v>
       </c>
@@ -10678,27 +10895,30 @@
       <c r="AP77" s="3">
         <v>0.21</v>
       </c>
-      <c r="AQ77" s="3">
+      <c r="AQ77" s="4">
+        <v>500</v>
+      </c>
+      <c r="AR77" s="3">
         <v>674</v>
       </c>
-      <c r="AR77" s="3">
+      <c r="AS77" s="3">
         <v>50</v>
       </c>
-      <c r="AS77" s="13">
+      <c r="AT77" s="13">
         <v>12.4</v>
       </c>
-      <c r="AT77" s="3">
+      <c r="AU77" s="3">
         <v>0.38</v>
       </c>
-      <c r="AU77" s="3">
+      <c r="AV77" s="3">
         <v>0.99</v>
       </c>
-      <c r="AV77" s="5">
-        <v>1</v>
-      </c>
-      <c r="AW77" s="13"/>
-    </row>
-    <row r="78" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW77" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX77" s="13"/>
+    </row>
+    <row r="78" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2</v>
       </c>
@@ -10793,22 +11013,25 @@
       <c r="AP78">
         <v>0.21</v>
       </c>
-      <c r="AQ78">
+      <c r="AQ78" s="2">
+        <v>500</v>
+      </c>
+      <c r="AR78">
         <v>674</v>
       </c>
-      <c r="AR78">
+      <c r="AS78">
         <v>50</v>
       </c>
-      <c r="AS78" s="16">
+      <c r="AT78" s="16">
         <v>-999</v>
       </c>
-      <c r="AT78">
+      <c r="AU78">
         <v>0.38</v>
       </c>
-      <c r="AU78">
+      <c r="AV78">
         <v>0.99</v>
       </c>
-      <c r="AV78" s="1">
+      <c r="AW78" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
StateTL revise celerity values 2/17/2022 - Issue #28
</commit_message>
<xml_diff>
--- a/matlab/StateTL_inputdata.xlsx
+++ b/matlab/StateTL_inputdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="SR" sheetId="13" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="evap" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1463,11 +1464,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="AJ26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" ySplit="1" topLeftCell="AA11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ43" sqref="AQ43"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,8 +1498,8 @@
     <col min="28" max="28" width="6.7109375" customWidth="1"/>
     <col min="29" max="29" width="5.85546875" customWidth="1"/>
     <col min="30" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.5703125" customWidth="1"/>
-    <col min="33" max="34" width="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.5703125" style="26" customWidth="1"/>
+    <col min="33" max="34" width="9" style="26" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9" style="2" customWidth="1"/>
     <col min="36" max="36" width="4.7109375" customWidth="1"/>
     <col min="37" max="37" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1601,13 +1602,13 @@
       <c r="AE1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AH1" s="24" t="s">
         <v>74</v>
       </c>
       <c r="AI1" s="4" t="s">
@@ -1710,14 +1711,14 @@
       <c r="AE2" s="17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF2" s="16">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="17">
-        <v>0.83</v>
-      </c>
-      <c r="AH2" s="17">
-        <v>0.21</v>
+      <c r="AF2" s="25">
+        <v>6</v>
+      </c>
+      <c r="AG2" s="25">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH2" s="25">
+        <v>0.2797</v>
       </c>
       <c r="AI2" s="16">
         <v>500</v>
@@ -1823,14 +1824,14 @@
       <c r="AE3" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="AH3" s="5">
-        <v>0.21</v>
+      <c r="AF3" s="24">
+        <v>6</v>
+      </c>
+      <c r="AG3" s="24">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH3" s="24">
+        <v>0.2797</v>
       </c>
       <c r="AI3" s="4">
         <v>500</v>
@@ -1937,14 +1938,14 @@
       <c r="AE4" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH4" s="1">
-        <v>0.21</v>
+      <c r="AF4" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG4" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH4" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI4" s="2">
         <v>500</v>
@@ -2049,14 +2050,14 @@
       <c r="AE5" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH5" s="1">
-        <v>0.21</v>
+      <c r="AF5" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG5" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH5" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI5" s="2">
         <v>500</v>
@@ -2160,14 +2161,14 @@
       <c r="AE6" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH6" s="1">
-        <v>0.21</v>
+      <c r="AF6" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG6" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH6" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI6" s="2">
         <v>500</v>
@@ -2271,14 +2272,14 @@
       <c r="AE7" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH7" s="1">
-        <v>0.21</v>
+      <c r="AF7" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG7" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH7" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI7" s="2">
         <v>500</v>
@@ -2382,14 +2383,14 @@
       <c r="AE8" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH8" s="1">
-        <v>0.21</v>
+      <c r="AF8" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG8" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH8" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI8" s="2">
         <v>500</v>
@@ -2491,14 +2492,14 @@
       <c r="AE9" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH9" s="1">
-        <v>0.21</v>
+      <c r="AF9" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG9" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH9" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI9" s="2">
         <v>500</v>
@@ -2609,14 +2610,14 @@
       <c r="AE10" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH10" s="1">
-        <v>0.21</v>
+      <c r="AF10" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG10" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH10" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI10" s="2">
         <v>500</v>
@@ -2720,14 +2721,14 @@
       <c r="AE11" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF11" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH11" s="1">
-        <v>0.21</v>
+      <c r="AF11" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG11" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH11" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI11" s="2">
         <v>500</v>
@@ -2835,14 +2836,14 @@
       <c r="AE12" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF12" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH12" s="1">
-        <v>0.21</v>
+      <c r="AF12" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG12" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH12" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI12" s="2">
         <v>500</v>
@@ -2943,14 +2944,14 @@
       <c r="AE13" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF13" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG13" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH13" s="1">
-        <v>0.21</v>
+      <c r="AF13" s="26">
+        <v>6</v>
+      </c>
+      <c r="AG13" s="26">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH13" s="26">
+        <v>0.2797</v>
       </c>
       <c r="AI13" s="2">
         <v>500</v>
@@ -3060,14 +3061,14 @@
       <c r="AE14" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF14" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG14" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="AH14" s="5">
-        <v>0.21</v>
+      <c r="AF14" s="24">
+        <v>6</v>
+      </c>
+      <c r="AG14" s="24">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AH14" s="24">
+        <v>0.2797</v>
       </c>
       <c r="AI14" s="4">
         <v>500</v>
@@ -3174,14 +3175,14 @@
       <c r="AE15" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF15" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG15" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH15" s="1">
-        <v>0.21</v>
+      <c r="AF15" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG15" s="26">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="AH15" s="26">
+        <v>0.22839999999999999</v>
       </c>
       <c r="AI15" s="2">
         <v>500</v>
@@ -3281,14 +3282,14 @@
       <c r="AE16" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF16" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG16" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH16" s="1">
-        <v>0.21</v>
+      <c r="AF16" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG16" s="26">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="AH16" s="26">
+        <v>0.22839999999999999</v>
       </c>
       <c r="AI16" s="2">
         <v>500</v>
@@ -3388,14 +3389,14 @@
       <c r="AE17" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG17" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH17" s="1">
-        <v>0.21</v>
+      <c r="AF17" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG17" s="26">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="AH17" s="26">
+        <v>0.22839999999999999</v>
       </c>
       <c r="AI17" s="2">
         <v>500</v>
@@ -3499,14 +3500,14 @@
       <c r="AE18" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF18" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG18" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH18" s="1">
-        <v>0.21</v>
+      <c r="AF18" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG18" s="26">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="AH18" s="26">
+        <v>0.22839999999999999</v>
       </c>
       <c r="AI18" s="2">
         <v>500</v>
@@ -3613,14 +3614,14 @@
       <c r="AE19" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF19" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG19" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH19" s="1">
-        <v>0.21</v>
+      <c r="AF19" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG19" s="26">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="AH19" s="26">
+        <v>0.22839999999999999</v>
       </c>
       <c r="AI19" s="2">
         <v>500</v>
@@ -3728,14 +3729,14 @@
       <c r="AE20" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF20" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG20" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH20" s="1">
-        <v>0.21</v>
+      <c r="AF20" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG20" s="26">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="AH20" s="26">
+        <v>0.22839999999999999</v>
       </c>
       <c r="AI20" s="2">
         <v>500</v>
@@ -3842,14 +3843,14 @@
       <c r="AE21" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF21" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG21" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="AH21" s="5">
-        <v>0.21</v>
+      <c r="AF21" s="24">
+        <v>4</v>
+      </c>
+      <c r="AG21" s="24">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="AH21" s="24">
+        <v>0.22839999999999999</v>
       </c>
       <c r="AI21" s="4">
         <v>500</v>
@@ -3953,14 +3954,14 @@
       <c r="AE22" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF22" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG22" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH22" s="1">
-        <v>0.21</v>
+      <c r="AF22" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG22" s="26">
+        <v>0.56440000000000001</v>
+      </c>
+      <c r="AH22" s="26">
+        <v>0.24690000000000001</v>
       </c>
       <c r="AI22" s="2">
         <v>500</v>
@@ -4062,14 +4063,14 @@
       <c r="AE23" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF23" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG23" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH23" s="1">
-        <v>0.21</v>
+      <c r="AF23" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG23" s="26">
+        <v>0.56440000000000001</v>
+      </c>
+      <c r="AH23" s="26">
+        <v>0.24690000000000001</v>
       </c>
       <c r="AI23" s="2">
         <v>500</v>
@@ -4177,14 +4178,14 @@
       <c r="AE24" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF24" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG24" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH24" s="1">
-        <v>0.21</v>
+      <c r="AF24" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG24" s="26">
+        <v>0.56440000000000001</v>
+      </c>
+      <c r="AH24" s="26">
+        <v>0.24690000000000001</v>
       </c>
       <c r="AI24" s="2">
         <v>500</v>
@@ -4296,14 +4297,14 @@
       <c r="AE25" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF25" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG25" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="AH25" s="5">
-        <v>0.21</v>
+      <c r="AF25" s="24">
+        <v>4</v>
+      </c>
+      <c r="AG25" s="24">
+        <v>0.56440000000000001</v>
+      </c>
+      <c r="AH25" s="24">
+        <v>0.24690000000000001</v>
       </c>
       <c r="AI25" s="4">
         <v>500</v>
@@ -4407,14 +4408,14 @@
       <c r="AE26" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF26" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG26" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH26" s="1">
-        <v>0.21</v>
+      <c r="AF26" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG26" s="26">
+        <v>0.70189999999999997</v>
+      </c>
+      <c r="AH26" s="26">
+        <v>0.2102</v>
       </c>
       <c r="AI26" s="2">
         <v>500</v>
@@ -4516,14 +4517,14 @@
       <c r="AE27" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF27" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG27" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH27" s="1">
-        <v>0.21</v>
+      <c r="AF27" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG27" s="26">
+        <v>0.70189999999999997</v>
+      </c>
+      <c r="AH27" s="26">
+        <v>0.2102</v>
       </c>
       <c r="AI27" s="2">
         <v>500</v>
@@ -4628,14 +4629,14 @@
       <c r="AE28" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF28" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG28" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH28" s="1">
-        <v>0.21</v>
+      <c r="AF28" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG28" s="26">
+        <v>0.70189999999999997</v>
+      </c>
+      <c r="AH28" s="26">
+        <v>0.2102</v>
       </c>
       <c r="AI28" s="2">
         <v>500</v>
@@ -4740,14 +4741,14 @@
       <c r="AE29" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF29" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG29" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH29" s="1">
-        <v>0.21</v>
+      <c r="AF29" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG29" s="26">
+        <v>0.70189999999999997</v>
+      </c>
+      <c r="AH29" s="26">
+        <v>0.2102</v>
       </c>
       <c r="AI29" s="2">
         <v>500</v>
@@ -4855,14 +4856,14 @@
       <c r="AE30" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF30" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG30" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH30" s="1">
-        <v>0.21</v>
+      <c r="AF30" s="26">
+        <v>4</v>
+      </c>
+      <c r="AG30" s="26">
+        <v>0.70189999999999997</v>
+      </c>
+      <c r="AH30" s="26">
+        <v>0.2102</v>
       </c>
       <c r="AI30" s="2">
         <v>500</v>
@@ -4977,14 +4978,14 @@
       <c r="AE31" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF31" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG31" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="AH31" s="5">
-        <v>0.21</v>
+      <c r="AF31" s="24">
+        <v>4</v>
+      </c>
+      <c r="AG31" s="24">
+        <v>0.70189999999999997</v>
+      </c>
+      <c r="AH31" s="24">
+        <v>0.2102</v>
       </c>
       <c r="AI31" s="4">
         <v>500</v>
@@ -5088,14 +5089,14 @@
       <c r="AE32" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF32" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG32" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH32" s="1">
-        <v>0.21</v>
+      <c r="AF32" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="AG32" s="26">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="AH32" s="26">
+        <v>0.2626</v>
       </c>
       <c r="AI32" s="2">
         <v>500</v>
@@ -5197,14 +5198,14 @@
       <c r="AE33" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG33" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH33" s="1">
-        <v>0.21</v>
+      <c r="AF33" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="AG33" s="26">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="AH33" s="26">
+        <v>0.2626</v>
       </c>
       <c r="AI33" s="2">
         <v>500</v>
@@ -5315,14 +5316,14 @@
       <c r="AE34" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG34" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH34" s="1">
-        <v>0.21</v>
+      <c r="AF34" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="AG34" s="26">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="AH34" s="26">
+        <v>0.2626</v>
       </c>
       <c r="AI34" s="2">
         <v>500</v>
@@ -5427,14 +5428,14 @@
       <c r="AE35" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF35" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG35" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH35" s="1">
-        <v>0.21</v>
+      <c r="AF35" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="AG35" s="26">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="AH35" s="26">
+        <v>0.2626</v>
       </c>
       <c r="AI35" s="2">
         <v>500</v>
@@ -5541,14 +5542,14 @@
       <c r="AE36" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF36" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG36" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="AH36" s="5">
-        <v>0.21</v>
+      <c r="AF36" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="AG36" s="24">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="AH36" s="24">
+        <v>0.2626</v>
       </c>
       <c r="AI36" s="4">
         <v>500</v>
@@ -5652,14 +5653,14 @@
       <c r="AE37" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF37" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG37" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH37" s="1">
-        <v>0.21</v>
+      <c r="AF37" s="26">
+        <v>3</v>
+      </c>
+      <c r="AG37" s="26">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH37" s="26">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI37" s="2">
         <v>500</v>
@@ -5759,14 +5760,14 @@
       <c r="AE38" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF38" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG38" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH38" s="1">
-        <v>0.21</v>
+      <c r="AF38" s="26">
+        <v>3</v>
+      </c>
+      <c r="AG38" s="26">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH38" s="26">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI38" s="2">
         <v>500</v>
@@ -5870,14 +5871,14 @@
       <c r="AE39" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF39" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG39" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH39" s="1">
-        <v>0.21</v>
+      <c r="AF39" s="26">
+        <v>3</v>
+      </c>
+      <c r="AG39" s="26">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH39" s="26">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI39" s="2">
         <v>500</v>
@@ -5983,14 +5984,14 @@
       <c r="AE40" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF40" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG40" s="5">
-        <v>0.83</v>
-      </c>
-      <c r="AH40" s="5">
-        <v>0.21</v>
+      <c r="AF40" s="24">
+        <v>3</v>
+      </c>
+      <c r="AG40" s="24">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH40" s="24">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI40" s="4">
         <v>500</v>
@@ -6094,14 +6095,14 @@
       <c r="AE41" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF41" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG41" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH41" s="1">
-        <v>0.21</v>
+      <c r="AF41" s="26">
+        <v>3</v>
+      </c>
+      <c r="AG41" s="26">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH41" s="26">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI41" s="2">
         <v>500</v>
@@ -6158,7 +6159,7 @@
         <v>64</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" ref="I42" si="9">IF(J42="Inflow",1,IF(J42="Outflow",-1,IF(J42="Gage",0,IF(J42="Top",0,""))))</f>
+        <f>IF(J42="Inflow",1,IF(J42="Outflow",-1,IF(J42="Gage",0,IF(J42="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J42" s="2" t="s">
@@ -6206,14 +6207,14 @@
       <c r="AE42" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF42" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG42" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH42" s="1">
-        <v>0.21</v>
+      <c r="AF42" s="26">
+        <v>3</v>
+      </c>
+      <c r="AG42" s="26">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH42" s="26">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI42" s="2">
         <v>500</v>
@@ -6277,7 +6278,7 @@
         <v>247</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" ref="I43" si="10">IF(J43="Inflow",1,IF(J43="Outflow",-1,IF(J43="Gage",0,IF(J43="Top",0,""))))</f>
+        <f>IF(J43="Inflow",1,IF(J43="Outflow",-1,IF(J43="Gage",0,IF(J43="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J43" s="2" t="s">
@@ -6321,14 +6322,14 @@
       <c r="AE43" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF43" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG43" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH43" s="1">
-        <v>0.21</v>
+      <c r="AF43" s="26">
+        <v>3</v>
+      </c>
+      <c r="AG43" s="26">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH43" s="26">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI43" s="2">
         <v>500</v>
@@ -6384,7 +6385,7 @@
         <v>274</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" ref="I44" si="11">IF(J44="Inflow",1,IF(J44="Outflow",-1,IF(J44="Gage",0,IF(J44="Top",0,""))))</f>
+        <f>IF(J44="Inflow",1,IF(J44="Outflow",-1,IF(J44="Gage",0,IF(J44="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J44" s="2" t="s">
@@ -6443,14 +6444,14 @@
       <c r="AE44" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF44" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG44" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="AH44" s="1">
-        <v>0.21</v>
+      <c r="AF44" s="26">
+        <v>3</v>
+      </c>
+      <c r="AG44" s="26">
+        <v>1.1425000000000001</v>
+      </c>
+      <c r="AH44" s="26">
+        <v>0.14080000000000001</v>
       </c>
       <c r="AI44" s="2">
         <v>500</v>
@@ -6501,9 +6502,9 @@
       <c r="Y45" s="21"/>
       <c r="AD45" s="7"/>
       <c r="AE45" s="21"/>
-      <c r="AF45" s="7"/>
-      <c r="AG45" s="21"/>
-      <c r="AH45" s="21"/>
+      <c r="AF45" s="27"/>
+      <c r="AG45" s="27"/>
+      <c r="AH45" s="27"/>
       <c r="AI45" s="7"/>
       <c r="AJ45" s="7"/>
       <c r="AL45" s="7"/>
@@ -6537,7 +6538,7 @@
         <v>192</v>
       </c>
       <c r="I46" s="50">
-        <f t="shared" ref="I46:I47" si="12">IF(J46="Inflow",1,IF(J46="Outflow",-1,IF(J46="Gage",0,IF(J46="Top",0,""))))</f>
+        <f>IF(J46="Inflow",1,IF(J46="Outflow",-1,IF(J46="Gage",0,IF(J46="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J46" s="50" t="s">
@@ -6592,14 +6593,14 @@
       <c r="AE46" s="51">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF46" s="50">
-        <v>1</v>
-      </c>
-      <c r="AG46" s="51">
-        <v>0.83</v>
-      </c>
-      <c r="AH46" s="51">
-        <v>0.21</v>
+      <c r="AF46" s="52">
+        <v>1</v>
+      </c>
+      <c r="AG46" s="52">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH46" s="52">
+        <v>0.1648</v>
       </c>
       <c r="AI46" s="50">
         <v>500</v>
@@ -6617,7 +6618,7 @@
         <v>251</v>
       </c>
       <c r="AN46" s="51">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO46" s="51">
         <v>1.32</v>
@@ -6654,7 +6655,7 @@
         <v>193</v>
       </c>
       <c r="I47" s="16">
-        <f t="shared" si="12"/>
+        <f>IF(J47="Inflow",1,IF(J47="Outflow",-1,IF(J47="Gage",0,IF(J47="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J47" s="16" t="s">
@@ -6707,14 +6708,14 @@
       <c r="AE47" s="17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF47" s="16">
-        <v>1</v>
-      </c>
-      <c r="AG47" s="17">
-        <v>0.83</v>
-      </c>
-      <c r="AH47" s="17">
-        <v>0.21</v>
+      <c r="AF47" s="25">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="25">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH47" s="25">
+        <v>0.1648</v>
       </c>
       <c r="AI47" s="16">
         <v>500</v>
@@ -6732,7 +6733,7 @@
         <v>251</v>
       </c>
       <c r="AN47" s="17">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO47" s="17">
         <v>1.32</v>
@@ -6775,9 +6776,9 @@
       </c>
       <c r="AD48" s="7"/>
       <c r="AE48" s="21"/>
-      <c r="AF48" s="7"/>
-      <c r="AG48" s="21"/>
-      <c r="AH48" s="21"/>
+      <c r="AF48" s="27"/>
+      <c r="AG48" s="27"/>
+      <c r="AH48" s="27"/>
       <c r="AI48" s="7"/>
       <c r="AJ48" s="7"/>
       <c r="AL48" s="7"/>
@@ -6811,7 +6812,7 @@
         <v>99</v>
       </c>
       <c r="I49" s="50">
-        <f t="shared" ref="I49:I51" si="13">IF(J49="Inflow",1,IF(J49="Outflow",-1,IF(J49="Gage",0,IF(J49="Top",0,""))))</f>
+        <f>IF(J49="Inflow",1,IF(J49="Outflow",-1,IF(J49="Gage",0,IF(J49="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J49" s="50" t="s">
@@ -6866,14 +6867,14 @@
       <c r="AE49" s="51">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF49" s="50">
-        <v>1</v>
-      </c>
-      <c r="AG49" s="51">
-        <v>0.83</v>
-      </c>
-      <c r="AH49" s="51">
-        <v>0.21</v>
+      <c r="AF49" s="52">
+        <v>1</v>
+      </c>
+      <c r="AG49" s="52">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH49" s="52">
+        <v>0.1648</v>
       </c>
       <c r="AI49" s="50">
         <v>500</v>
@@ -6891,7 +6892,7 @@
         <v>251</v>
       </c>
       <c r="AN49" s="51">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO49" s="51">
         <v>1.32</v>
@@ -6927,7 +6928,7 @@
         <v>101</v>
       </c>
       <c r="I50" s="16">
-        <f t="shared" si="13"/>
+        <f>IF(J50="Inflow",1,IF(J50="Outflow",-1,IF(J50="Gage",0,IF(J50="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J50" s="16" t="s">
@@ -6954,7 +6955,7 @@
       </c>
       <c r="U50" s="17"/>
       <c r="V50" s="17">
-        <f t="shared" ref="V50:V51" si="14">Y$52/SUM(Y$49:Y$51)</f>
+        <f>Y$52/SUM(Y$49:Y$51)</f>
         <v>0.16300081998869265</v>
       </c>
       <c r="W50" s="25"/>
@@ -6980,14 +6981,14 @@
       <c r="AE50" s="17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF50" s="16">
-        <v>1</v>
-      </c>
-      <c r="AG50" s="17">
-        <v>0.83</v>
-      </c>
-      <c r="AH50" s="17">
-        <v>0.21</v>
+      <c r="AF50" s="25">
+        <v>1</v>
+      </c>
+      <c r="AG50" s="25">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH50" s="25">
+        <v>0.1648</v>
       </c>
       <c r="AI50" s="16">
         <v>500</v>
@@ -7005,7 +7006,7 @@
         <v>251</v>
       </c>
       <c r="AN50" s="17">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO50" s="17">
         <v>1.32</v>
@@ -7041,7 +7042,7 @@
         <v>102</v>
       </c>
       <c r="I51" s="7">
-        <f t="shared" si="13"/>
+        <f>IF(J51="Inflow",1,IF(J51="Outflow",-1,IF(J51="Gage",0,IF(J51="Top",0,""))))</f>
         <v>-1</v>
       </c>
       <c r="J51" s="7" t="s">
@@ -7064,7 +7065,7 @@
       </c>
       <c r="U51" s="21"/>
       <c r="V51" s="21">
-        <f t="shared" si="14"/>
+        <f>Y$52/SUM(Y$49:Y$51)</f>
         <v>0.16300081998869265</v>
       </c>
       <c r="W51" s="27"/>
@@ -7090,14 +7091,14 @@
       <c r="AE51" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF51" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG51" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="AH51" s="21">
-        <v>0.21</v>
+      <c r="AF51" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="27">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH51" s="27">
+        <v>0.1648</v>
       </c>
       <c r="AI51" s="7">
         <v>500</v>
@@ -7115,7 +7116,7 @@
         <v>251</v>
       </c>
       <c r="AN51" s="21">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO51" s="21">
         <v>1.32</v>
@@ -7153,9 +7154,9 @@
       </c>
       <c r="AD52" s="7"/>
       <c r="AE52" s="21"/>
-      <c r="AF52" s="7"/>
-      <c r="AG52" s="21"/>
-      <c r="AH52" s="21"/>
+      <c r="AF52" s="27"/>
+      <c r="AG52" s="27"/>
+      <c r="AH52" s="27"/>
       <c r="AI52" s="7"/>
       <c r="AJ52" s="7"/>
       <c r="AL52" s="7"/>
@@ -7191,7 +7192,7 @@
         <v>258</v>
       </c>
       <c r="I53" s="50">
-        <f t="shared" ref="I53:I55" si="15">IF(J53="Inflow",1,IF(J53="Outflow",-1,IF(J53="Gage",0,IF(J53="Top",0,""))))</f>
+        <f>IF(J53="Inflow",1,IF(J53="Outflow",-1,IF(J53="Gage",0,IF(J53="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J53" s="50" t="s">
@@ -7251,14 +7252,14 @@
       <c r="AE53" s="51">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF53" s="50">
-        <v>1</v>
-      </c>
-      <c r="AG53" s="51">
-        <v>0.83</v>
-      </c>
-      <c r="AH53" s="51">
-        <v>0.21</v>
+      <c r="AF53" s="52">
+        <v>1</v>
+      </c>
+      <c r="AG53" s="52">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH53" s="52">
+        <v>0.1648</v>
       </c>
       <c r="AI53" s="50">
         <v>500</v>
@@ -7276,7 +7277,7 @@
         <v>251</v>
       </c>
       <c r="AN53" s="51">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO53" s="51">
         <v>1.32</v>
@@ -7312,7 +7313,7 @@
         <v>260</v>
       </c>
       <c r="I54" s="16">
-        <f t="shared" si="15"/>
+        <f>IF(J54="Inflow",1,IF(J54="Outflow",-1,IF(J54="Gage",0,IF(J54="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J54" s="16" t="s">
@@ -7339,7 +7340,7 @@
       </c>
       <c r="U54" s="17"/>
       <c r="V54" s="17">
-        <f t="shared" ref="V54:V55" si="16">Y$56/SUM(W$53,Y$53:Y$55)</f>
+        <f>Y$56/SUM(W$53,Y$53:Y$55)</f>
         <v>0.41087026574215463</v>
       </c>
       <c r="W54" s="25"/>
@@ -7365,14 +7366,14 @@
       <c r="AE54" s="17">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF54" s="16">
-        <v>1</v>
-      </c>
-      <c r="AG54" s="17">
-        <v>0.83</v>
-      </c>
-      <c r="AH54" s="17">
-        <v>0.21</v>
+      <c r="AF54" s="25">
+        <v>1</v>
+      </c>
+      <c r="AG54" s="25">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH54" s="25">
+        <v>0.1648</v>
       </c>
       <c r="AI54" s="16">
         <v>500</v>
@@ -7390,7 +7391,7 @@
         <v>251</v>
       </c>
       <c r="AN54" s="17">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO54" s="17">
         <v>1.32</v>
@@ -7426,7 +7427,7 @@
         <v>262</v>
       </c>
       <c r="I55" s="7">
-        <f t="shared" si="15"/>
+        <f>IF(J55="Inflow",1,IF(J55="Outflow",-1,IF(J55="Gage",0,IF(J55="Top",0,""))))</f>
         <v>-1</v>
       </c>
       <c r="J55" s="7" t="s">
@@ -7449,7 +7450,7 @@
       </c>
       <c r="U55" s="21"/>
       <c r="V55" s="21">
-        <f t="shared" si="16"/>
+        <f>Y$56/SUM(W$53,Y$53:Y$55)</f>
         <v>0.41087026574215463</v>
       </c>
       <c r="W55" s="27"/>
@@ -7475,14 +7476,14 @@
       <c r="AE55" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF55" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG55" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="AH55" s="21">
-        <v>0.21</v>
+      <c r="AF55" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG55" s="27">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH55" s="27">
+        <v>0.1648</v>
       </c>
       <c r="AI55" s="7">
         <v>500</v>
@@ -7500,7 +7501,7 @@
         <v>251</v>
       </c>
       <c r="AN55" s="21">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO55" s="21">
         <v>1.32</v>
@@ -7538,9 +7539,9 @@
       </c>
       <c r="AD56" s="7"/>
       <c r="AE56" s="21"/>
-      <c r="AF56" s="7"/>
-      <c r="AG56" s="21"/>
-      <c r="AH56" s="21"/>
+      <c r="AF56" s="27"/>
+      <c r="AG56" s="27"/>
+      <c r="AH56" s="27"/>
       <c r="AI56" s="7"/>
       <c r="AJ56" s="7"/>
       <c r="AL56" s="7"/>
@@ -7574,7 +7575,7 @@
         <v>267</v>
       </c>
       <c r="I57" s="42">
-        <f t="shared" ref="I57:I59" si="17">IF(J57="Inflow",1,IF(J57="Outflow",-1,IF(J57="Gage",0,IF(J57="Top",0,""))))</f>
+        <f>IF(J57="Inflow",1,IF(J57="Outflow",-1,IF(J57="Gage",0,IF(J57="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J57" s="42" t="s">
@@ -7627,14 +7628,14 @@
       <c r="AE57" s="44">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF57" s="42">
-        <v>1</v>
-      </c>
-      <c r="AG57" s="44">
-        <v>0.83</v>
-      </c>
-      <c r="AH57" s="44">
-        <v>0.21</v>
+      <c r="AF57" s="43">
+        <v>1</v>
+      </c>
+      <c r="AG57" s="43">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH57" s="43">
+        <v>0.1648</v>
       </c>
       <c r="AI57" s="42">
         <v>500</v>
@@ -7652,7 +7653,7 @@
         <v>251</v>
       </c>
       <c r="AN57" s="44">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO57" s="44">
         <v>1.32</v>
@@ -7690,7 +7691,7 @@
         <v>264</v>
       </c>
       <c r="I58" s="7">
-        <f t="shared" ref="I58" si="18">IF(J58="Inflow",1,IF(J58="Outflow",-1,IF(J58="Gage",0,IF(J58="Top",0,""))))</f>
+        <f>IF(J58="Inflow",1,IF(J58="Outflow",-1,IF(J58="Gage",0,IF(J58="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J58" s="7" t="s">
@@ -7750,14 +7751,14 @@
       <c r="AE58" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF58" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG58" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="AH58" s="21">
-        <v>0.21</v>
+      <c r="AF58" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG58" s="27">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH58" s="27">
+        <v>0.1648</v>
       </c>
       <c r="AI58" s="7">
         <v>500</v>
@@ -7775,7 +7776,7 @@
         <v>251</v>
       </c>
       <c r="AN58" s="21">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO58" s="21">
         <v>1.32</v>
@@ -7811,7 +7812,7 @@
         <v>268</v>
       </c>
       <c r="I59" s="7">
-        <f t="shared" si="17"/>
+        <f>IF(J59="Inflow",1,IF(J59="Outflow",-1,IF(J59="Gage",0,IF(J59="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J59" s="7" t="s">
@@ -7871,14 +7872,14 @@
       <c r="AE59" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF59" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG59" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="AH59" s="21">
-        <v>0.21</v>
+      <c r="AF59" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG59" s="27">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH59" s="27">
+        <v>0.1648</v>
       </c>
       <c r="AI59" s="7">
         <v>500</v>
@@ -7896,7 +7897,7 @@
         <v>251</v>
       </c>
       <c r="AN59" s="21">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AO59" s="21">
         <v>1.32</v>
@@ -7934,9 +7935,9 @@
       </c>
       <c r="AD60" s="7"/>
       <c r="AE60" s="21"/>
-      <c r="AF60" s="7"/>
-      <c r="AG60" s="21"/>
-      <c r="AH60" s="21"/>
+      <c r="AF60" s="27"/>
+      <c r="AG60" s="27"/>
+      <c r="AH60" s="27"/>
       <c r="AI60" s="7"/>
       <c r="AJ60" s="7"/>
       <c r="AL60" s="7"/>
@@ -7970,7 +7971,7 @@
         <v>107</v>
       </c>
       <c r="I61" s="42">
-        <f t="shared" ref="I61:I62" si="19">IF(J61="Inflow",1,IF(J61="Outflow",-1,IF(J61="Gage",0,IF(J61="Top",0,""))))</f>
+        <f>IF(J61="Inflow",1,IF(J61="Outflow",-1,IF(J61="Gage",0,IF(J61="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J61" s="42" t="s">
@@ -8018,14 +8019,14 @@
       <c r="AE61" s="44">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF61" s="42">
-        <v>1</v>
-      </c>
-      <c r="AG61" s="44">
-        <v>0.83</v>
-      </c>
-      <c r="AH61" s="44">
-        <v>0.21</v>
+      <c r="AF61" s="43">
+        <v>1</v>
+      </c>
+      <c r="AG61" s="43">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH61" s="43">
+        <v>0.1648</v>
       </c>
       <c r="AI61" s="42">
         <v>500</v>
@@ -8079,7 +8080,7 @@
         <v>109</v>
       </c>
       <c r="I62" s="7">
-        <f t="shared" si="19"/>
+        <f>IF(J62="Inflow",1,IF(J62="Outflow",-1,IF(J62="Gage",0,IF(J62="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J62" s="7" t="s">
@@ -8131,14 +8132,14 @@
       <c r="AE62" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF62" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG62" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="AH62" s="21">
-        <v>0.21</v>
+      <c r="AF62" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG62" s="27">
+        <v>1.1377999999999999</v>
+      </c>
+      <c r="AH62" s="27">
+        <v>0.1648</v>
       </c>
       <c r="AI62" s="7">
         <v>500</v>
@@ -8196,9 +8197,9 @@
       <c r="AC63" s="38"/>
       <c r="AD63" s="38"/>
       <c r="AE63" s="38"/>
-      <c r="AF63" s="47"/>
-      <c r="AG63" s="38"/>
-      <c r="AH63" s="38"/>
+      <c r="AF63" s="46"/>
+      <c r="AG63" s="46"/>
+      <c r="AH63" s="46"/>
       <c r="AI63" s="47"/>
       <c r="AJ63" s="47"/>
       <c r="AK63" s="38"/>
@@ -8233,7 +8234,7 @@
         <v>111</v>
       </c>
       <c r="I64" s="7">
-        <f t="shared" ref="I64:I66" si="20">IF(J64="Inflow",1,IF(J64="Outflow",-1,IF(J64="Gage",0,IF(J64="Top",0,""))))</f>
+        <f>IF(J64="Inflow",1,IF(J64="Outflow",-1,IF(J64="Gage",0,IF(J64="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J64" s="2" t="s">
@@ -8287,13 +8288,13 @@
       <c r="AE64" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF64" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG64" s="21">
+      <c r="AF64" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG64" s="27">
         <v>0.83</v>
       </c>
-      <c r="AH64" s="21">
+      <c r="AH64" s="27">
         <v>0.21</v>
       </c>
       <c r="AI64" s="7">
@@ -8347,7 +8348,7 @@
         <v>112</v>
       </c>
       <c r="I65" s="7">
-        <f t="shared" si="20"/>
+        <f>IF(J65="Inflow",1,IF(J65="Outflow",-1,IF(J65="Gage",0,IF(J65="Top",0,""))))</f>
         <v>-1</v>
       </c>
       <c r="J65" s="7" t="s">
@@ -8399,13 +8400,13 @@
       <c r="AE65" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF65" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG65" s="21">
+      <c r="AF65" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG65" s="27">
         <v>0.83</v>
       </c>
-      <c r="AH65" s="21">
+      <c r="AH65" s="27">
         <v>0.21</v>
       </c>
       <c r="AI65" s="7">
@@ -8459,7 +8460,7 @@
         <v>113</v>
       </c>
       <c r="I66" s="7">
-        <f t="shared" si="20"/>
+        <f>IF(J66="Inflow",1,IF(J66="Outflow",-1,IF(J66="Gage",0,IF(J66="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J66" s="7" t="s">
@@ -8509,13 +8510,13 @@
       <c r="AE66" s="21">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF66" s="7">
-        <v>1</v>
-      </c>
-      <c r="AG66" s="21">
+      <c r="AF66" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG66" s="27">
         <v>0.83</v>
       </c>
-      <c r="AH66" s="21">
+      <c r="AH66" s="27">
         <v>0.21</v>
       </c>
       <c r="AI66" s="7">
@@ -8562,6 +8563,9 @@
       <c r="W67" s="46"/>
       <c r="X67" s="36"/>
       <c r="Y67" s="36"/>
+      <c r="AF67" s="35"/>
+      <c r="AG67" s="35"/>
+      <c r="AH67" s="35"/>
       <c r="AI67" s="34"/>
       <c r="AJ67" s="34"/>
       <c r="AL67" s="34"/>
@@ -8592,7 +8596,7 @@
         <v>114</v>
       </c>
       <c r="I68" s="6">
-        <f t="shared" ref="I68:I71" si="21">IF(J68="Inflow",1,IF(J68="Outflow",-1,IF(J68="Gage",0,IF(J68="Top",0,""))))</f>
+        <f>IF(J68="Inflow",1,IF(J68="Outflow",-1,IF(J68="Gage",0,IF(J68="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J68" s="6" t="s">
@@ -8642,13 +8646,13 @@
       <c r="AE68" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF68" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG68" s="6">
+      <c r="AF68" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG68" s="27">
         <v>0.83</v>
       </c>
-      <c r="AH68" s="6">
+      <c r="AH68" s="27">
         <v>0.21</v>
       </c>
       <c r="AI68" s="7">
@@ -8703,7 +8707,7 @@
         <v>109</v>
       </c>
       <c r="I69" s="6">
-        <f t="shared" si="21"/>
+        <f>IF(J69="Inflow",1,IF(J69="Outflow",-1,IF(J69="Gage",0,IF(J69="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J69" s="6" t="s">
@@ -8749,13 +8753,13 @@
       <c r="AE69" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF69" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG69" s="6">
+      <c r="AF69" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG69" s="27">
         <v>0.83</v>
       </c>
-      <c r="AH69" s="6">
+      <c r="AH69" s="27">
         <v>0.21</v>
       </c>
       <c r="AI69" s="7">
@@ -8807,7 +8811,7 @@
         <v>116</v>
       </c>
       <c r="I70" s="6">
-        <f t="shared" si="21"/>
+        <f>IF(J70="Inflow",1,IF(J70="Outflow",-1,IF(J70="Gage",0,IF(J70="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J70" s="6" t="s">
@@ -8857,13 +8861,13 @@
       <c r="AE70" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF70" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG70" s="6">
+      <c r="AF70" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG70" s="27">
         <v>0.83</v>
       </c>
-      <c r="AH70" s="6">
+      <c r="AH70" s="27">
         <v>0.21</v>
       </c>
       <c r="AI70" s="7">
@@ -8915,7 +8919,7 @@
         <v>119</v>
       </c>
       <c r="I71" s="7">
-        <f t="shared" si="21"/>
+        <f>IF(J71="Inflow",1,IF(J71="Outflow",-1,IF(J71="Gage",0,IF(J71="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J71" s="7" t="s">
@@ -8965,13 +8969,13 @@
       <c r="AE71" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF71" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG71" s="6">
+      <c r="AF71" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG71" s="27">
         <v>0.83</v>
       </c>
-      <c r="AH71" s="6">
+      <c r="AH71" s="27">
         <v>0.21</v>
       </c>
       <c r="AI71" s="7">
@@ -9011,6 +9015,9 @@
       <c r="P72" s="35"/>
       <c r="V72" s="37"/>
       <c r="W72" s="35"/>
+      <c r="AF72" s="35"/>
+      <c r="AG72" s="35"/>
+      <c r="AH72" s="35"/>
       <c r="AI72" s="34"/>
       <c r="AL72" s="34"/>
       <c r="AM72" s="34"/>
@@ -9040,7 +9047,7 @@
         <v>160</v>
       </c>
       <c r="I73" s="7">
-        <f t="shared" ref="I73:I92" si="22">IF(J73="Inflow",1,IF(J73="Outflow",-1,IF(J73="Gage",0,IF(J73="Top",0,""))))</f>
+        <f t="shared" ref="I73:I92" si="9">IF(J73="Inflow",1,IF(J73="Outflow",-1,IF(J73="Gage",0,IF(J73="Top",0,""))))</f>
         <v>0</v>
       </c>
       <c r="J73" t="s">
@@ -9090,14 +9097,14 @@
       <c r="AE73">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF73">
-        <v>1</v>
-      </c>
-      <c r="AG73">
-        <v>0.83</v>
-      </c>
-      <c r="AH73">
-        <v>0.21</v>
+      <c r="AF73" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG73" s="26">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH73" s="26">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI73" s="2">
         <v>500</v>
@@ -9149,7 +9156,7 @@
         <v>159</v>
       </c>
       <c r="I74" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J74" s="15" t="s">
@@ -9197,14 +9204,14 @@
       <c r="AE74" s="15">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF74" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG74" s="15">
-        <v>0.83</v>
-      </c>
-      <c r="AH74" s="15">
-        <v>0.21</v>
+      <c r="AF74" s="25">
+        <v>1</v>
+      </c>
+      <c r="AG74" s="25">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH74" s="25">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI74" s="16">
         <v>500</v>
@@ -9247,7 +9254,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="6">
-        <f t="shared" ref="E75:E92" si="23">E74+1</f>
+        <f t="shared" ref="E75:E92" si="10">E74+1</f>
         <v>3</v>
       </c>
       <c r="F75" s="7">
@@ -9258,7 +9265,7 @@
         <v>149</v>
       </c>
       <c r="I75" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J75" s="6" t="s">
@@ -9305,14 +9312,14 @@
       <c r="AE75" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF75" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG75" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH75" s="6">
-        <v>0.21</v>
+      <c r="AF75" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG75" s="27">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH75" s="27">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI75" s="7">
         <v>500</v>
@@ -9351,11 +9358,11 @@
         <v>2</v>
       </c>
       <c r="D76" s="6">
-        <f t="shared" ref="D76:D91" si="24">D75+1</f>
+        <f t="shared" ref="D76:D91" si="11">D75+1</f>
         <v>3</v>
       </c>
       <c r="E76" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="F76" s="7">
@@ -9366,7 +9373,7 @@
         <v>148</v>
       </c>
       <c r="I76" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J76" s="6" t="s">
@@ -9407,14 +9414,14 @@
       <c r="AE76" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF76" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG76" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH76" s="6">
-        <v>0.21</v>
+      <c r="AF76" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG76" s="27">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH76" s="27">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI76" s="7">
         <v>500</v>
@@ -9453,11 +9460,11 @@
         <v>2</v>
       </c>
       <c r="D77" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="E77" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="F77" s="26">
@@ -9470,7 +9477,7 @@
         <v>290</v>
       </c>
       <c r="I77" s="7">
-        <f t="shared" ref="I77" si="25">IF(J77="Inflow",1,IF(J77="Outflow",-1,IF(J77="Gage",0,IF(J77="Top",0,""))))</f>
+        <f>IF(J77="Inflow",1,IF(J77="Outflow",-1,IF(J77="Gage",0,IF(J77="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J77" t="s">
@@ -9530,14 +9537,14 @@
       <c r="AE77" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF77" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG77" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH77" s="6">
-        <v>0.21</v>
+      <c r="AF77" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG77" s="27">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH77" s="27">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI77" s="7">
         <v>500</v>
@@ -9576,11 +9583,11 @@
         <v>2</v>
       </c>
       <c r="D78" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E78" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="F78" s="26">
@@ -9593,7 +9600,7 @@
         <v>289</v>
       </c>
       <c r="I78" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J78" t="s">
@@ -9653,14 +9660,14 @@
       <c r="AE78" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF78" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG78" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH78" s="6">
-        <v>0.21</v>
+      <c r="AF78" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG78" s="27">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH78" s="27">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI78" s="7">
         <v>500</v>
@@ -9699,11 +9706,11 @@
         <v>2</v>
       </c>
       <c r="D79" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="E79" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="F79" s="26">
@@ -9716,7 +9723,7 @@
         <v>288</v>
       </c>
       <c r="I79" s="7">
-        <f t="shared" ref="I79" si="26">IF(J79="Inflow",1,IF(J79="Outflow",-1,IF(J79="Gage",0,IF(J79="Top",0,""))))</f>
+        <f>IF(J79="Inflow",1,IF(J79="Outflow",-1,IF(J79="Gage",0,IF(J79="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J79" t="s">
@@ -9776,14 +9783,14 @@
       <c r="AE79" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF79" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG79" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH79" s="6">
-        <v>0.21</v>
+      <c r="AF79" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG79" s="27">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH79" s="27">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI79" s="7">
         <v>500</v>
@@ -9822,11 +9829,11 @@
         <v>2</v>
       </c>
       <c r="D80" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E80" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="F80" s="7">
@@ -9837,7 +9844,7 @@
         <v>150</v>
       </c>
       <c r="I80" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J80" s="6" t="s">
@@ -9885,14 +9892,14 @@
       <c r="AE80" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF80" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG80" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH80" s="6">
-        <v>0.21</v>
+      <c r="AF80" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG80" s="27">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH80" s="27">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI80" s="7">
         <v>500</v>
@@ -9931,11 +9938,11 @@
         <v>2</v>
       </c>
       <c r="D81" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="E81" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="F81" s="7">
@@ -9948,7 +9955,7 @@
         <v>292</v>
       </c>
       <c r="I81" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J81" t="s">
@@ -10008,14 +10015,14 @@
       <c r="AE81" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF81" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG81" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH81" s="6">
-        <v>0.21</v>
+      <c r="AF81" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG81" s="27">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH81" s="27">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI81" s="7">
         <v>500</v>
@@ -10054,11 +10061,11 @@
         <v>2</v>
       </c>
       <c r="D82" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="E82" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="F82" s="4">
@@ -10069,7 +10076,7 @@
         <v>151</v>
       </c>
       <c r="I82" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J82" s="3" t="s">
@@ -10119,14 +10126,14 @@
       <c r="AE82" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF82" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG82" s="3">
-        <v>0.83</v>
-      </c>
-      <c r="AH82" s="3">
-        <v>0.21</v>
+      <c r="AF82" s="24">
+        <v>1</v>
+      </c>
+      <c r="AG82" s="24">
+        <v>0.98509999999999998</v>
+      </c>
+      <c r="AH82" s="24">
+        <v>0.20039999999999999</v>
       </c>
       <c r="AI82" s="4">
         <v>500</v>
@@ -10168,7 +10175,7 @@
         <v>1</v>
       </c>
       <c r="E83">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="F83" s="2">
@@ -10178,7 +10185,7 @@
         <v>144</v>
       </c>
       <c r="I83" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J83" t="s">
@@ -10227,14 +10234,14 @@
       <c r="AE83">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF83">
-        <v>1</v>
-      </c>
-      <c r="AG83">
+      <c r="AF83" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG83" s="26">
         <v>0.83</v>
       </c>
-      <c r="AH83">
-        <v>0.21</v>
+      <c r="AH83" s="26">
+        <v>0.2</v>
       </c>
       <c r="AI83" s="2">
         <v>500</v>
@@ -10272,11 +10279,11 @@
         <v>3</v>
       </c>
       <c r="D84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="E84">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="F84" s="2">
@@ -10286,7 +10293,7 @@
         <v>152</v>
       </c>
       <c r="I84" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J84" t="s">
@@ -10335,14 +10342,14 @@
       <c r="AE84">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF84">
-        <v>1</v>
-      </c>
-      <c r="AG84">
+      <c r="AF84" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG84" s="26">
         <v>0.83</v>
       </c>
-      <c r="AH84">
-        <v>0.21</v>
+      <c r="AH84" s="26">
+        <v>0.2</v>
       </c>
       <c r="AI84" s="2">
         <v>500</v>
@@ -10380,11 +10387,11 @@
         <v>3</v>
       </c>
       <c r="D85">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E85">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="F85" s="2">
@@ -10397,7 +10404,7 @@
         <v>295</v>
       </c>
       <c r="I85" s="7">
-        <f t="shared" ref="I85" si="27">IF(J85="Inflow",1,IF(J85="Outflow",-1,IF(J85="Gage",0,IF(J85="Top",0,""))))</f>
+        <f>IF(J85="Inflow",1,IF(J85="Outflow",-1,IF(J85="Gage",0,IF(J85="Top",0,""))))</f>
         <v>1</v>
       </c>
       <c r="J85" t="s">
@@ -10456,14 +10463,14 @@
       <c r="AE85">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF85">
-        <v>1</v>
-      </c>
-      <c r="AG85">
+      <c r="AF85" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG85" s="26">
         <v>0.83</v>
       </c>
-      <c r="AH85">
-        <v>0.21</v>
+      <c r="AH85" s="26">
+        <v>0.2</v>
       </c>
       <c r="AI85" s="2">
         <v>500</v>
@@ -10501,11 +10508,11 @@
         <v>3</v>
       </c>
       <c r="D86">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="E86">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="F86" s="2">
@@ -10518,7 +10525,7 @@
         <v>145</v>
       </c>
       <c r="I86" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J86" t="s">
@@ -10567,14 +10574,14 @@
       <c r="AE86">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF86">
-        <v>1</v>
-      </c>
-      <c r="AG86">
+      <c r="AF86" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG86" s="26">
         <v>0.83</v>
       </c>
-      <c r="AH86">
-        <v>0.21</v>
+      <c r="AH86" s="26">
+        <v>0.2</v>
       </c>
       <c r="AI86" s="2">
         <v>500</v>
@@ -10612,11 +10619,11 @@
         <v>3</v>
       </c>
       <c r="D87">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E87">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
       <c r="F87" s="2">
@@ -10629,7 +10636,7 @@
         <v>153</v>
       </c>
       <c r="I87" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J87" t="s">
@@ -10672,14 +10679,14 @@
       <c r="AE87">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF87">
-        <v>1</v>
-      </c>
-      <c r="AG87">
+      <c r="AF87" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG87" s="26">
         <v>0.83</v>
       </c>
-      <c r="AH87">
-        <v>0.21</v>
+      <c r="AH87" s="26">
+        <v>0.2</v>
       </c>
       <c r="AI87" s="2">
         <v>500</v>
@@ -10720,11 +10727,11 @@
         <v>3</v>
       </c>
       <c r="D88">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="E88">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="F88" s="2">
@@ -10734,7 +10741,7 @@
         <v>154</v>
       </c>
       <c r="I88" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J88" t="s">
@@ -10783,14 +10790,14 @@
       <c r="AE88">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF88">
-        <v>1</v>
-      </c>
-      <c r="AG88">
+      <c r="AF88" s="26">
+        <v>1</v>
+      </c>
+      <c r="AG88" s="26">
         <v>0.83</v>
       </c>
-      <c r="AH88">
-        <v>0.21</v>
+      <c r="AH88" s="26">
+        <v>0.2</v>
       </c>
       <c r="AI88" s="2">
         <v>500</v>
@@ -10831,7 +10838,7 @@
         <v>1</v>
       </c>
       <c r="E89" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
       <c r="F89" s="16">
@@ -10842,7 +10849,7 @@
         <v>146</v>
       </c>
       <c r="I89" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J89" s="15" t="s">
@@ -10889,14 +10896,14 @@
       <c r="AE89" s="15">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF89" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG89" s="15">
-        <v>0.83</v>
-      </c>
-      <c r="AH89" s="15">
-        <v>0.21</v>
+      <c r="AF89" s="25">
+        <v>1</v>
+      </c>
+      <c r="AG89" s="25">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="AH89" s="25">
+        <v>0.19439999999999999</v>
       </c>
       <c r="AI89" s="16">
         <v>500</v>
@@ -10935,11 +10942,11 @@
         <v>4</v>
       </c>
       <c r="D90" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="E90" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="F90" s="7">
@@ -10950,7 +10957,7 @@
         <v>155</v>
       </c>
       <c r="I90" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J90" s="6" t="s">
@@ -10994,14 +11001,14 @@
       <c r="AE90" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF90" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG90" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="AH90" s="6">
-        <v>0.21</v>
+      <c r="AF90" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG90" s="27">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="AH90" s="27">
+        <v>0.19439999999999999</v>
       </c>
       <c r="AI90" s="7">
         <v>500</v>
@@ -11040,11 +11047,11 @@
         <v>4</v>
       </c>
       <c r="D91" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E91" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>19</v>
       </c>
       <c r="F91" s="4">
@@ -11057,7 +11064,7 @@
         <v>156</v>
       </c>
       <c r="I91" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="J91" s="3" t="s">
@@ -11110,14 +11117,14 @@
       <c r="AE91" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF91" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG91" s="3">
-        <v>0.83</v>
-      </c>
-      <c r="AH91" s="3">
-        <v>0.21</v>
+      <c r="AF91" s="24">
+        <v>1</v>
+      </c>
+      <c r="AG91" s="24">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="AH91" s="24">
+        <v>0.19439999999999999</v>
       </c>
       <c r="AI91" s="4">
         <v>500</v>
@@ -11159,7 +11166,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="F92" s="16">
@@ -11170,7 +11177,7 @@
         <v>147</v>
       </c>
       <c r="I92" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J92" s="15" t="s">
@@ -11226,14 +11233,14 @@
       <c r="AE92" s="15">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AF92" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG92" s="15">
-        <v>0.83</v>
-      </c>
-      <c r="AH92" s="15">
-        <v>0.21</v>
+      <c r="AF92" s="25">
+        <v>1</v>
+      </c>
+      <c r="AG92" s="25">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="AH92" s="25">
+        <v>0.19439999999999999</v>
       </c>
       <c r="AI92" s="16">
         <v>500</v>
@@ -11275,6 +11282,9 @@
       <c r="P93" s="35"/>
       <c r="V93" s="37"/>
       <c r="W93" s="35"/>
+      <c r="AF93" s="35"/>
+      <c r="AG93" s="35"/>
+      <c r="AH93" s="35"/>
       <c r="AI93" s="34"/>
       <c r="AL93" s="34"/>
       <c r="AM93" s="34"/>
@@ -18957,7 +18967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19209,7 +19219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>